<commit_message>
Add columns for tool results
</commit_message>
<xml_diff>
--- a/DotNET Tests and Results.xlsx
+++ b/DotNET Tests and Results.xlsx
@@ -14,12 +14,12 @@
     <sheet name="Contrast Results for XXE" sheetId="3" r:id="rId5"/>
     <sheet name="Contrast Results for HQL" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="126">
   <si>
     <t>XML Parser</t>
   </si>
@@ -477,6 +477,33 @@
   </si>
   <si>
     <t>HQL/SQL Injection</t>
+  </si>
+  <si>
+    <t>Fortify Detection</t>
+  </si>
+  <si>
+    <t>Contrast Detection</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>Fail</t>
+  </si>
+  <si>
+    <t>Fortify Detection (.NET 4.5.1)</t>
+  </si>
+  <si>
+    <t>Contrast Detection (4.5.1)</t>
+  </si>
+  <si>
+    <t>Contrast Detection (4.5.2)</t>
+  </si>
+  <si>
+    <t>Fortify Detection (4.5.2)</t>
   </si>
 </sst>
 </file>
@@ -664,7 +691,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -687,15 +714,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -719,16 +737,1948 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="2" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="2" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Total" xfId="1" builtinId="25"/>
   </cellStyles>
-  <dxfs count="56">
+  <dxfs count="231">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -746,84 +2696,68 @@
       </border>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="double">
+          <color theme="4"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="double">
+          <color theme="4"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="double">
+          <color theme="4"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="double">
+          <color theme="4"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -1022,13 +2956,6 @@
         <top style="thin">
           <color theme="4" tint="0.39997558519241921"/>
         </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -1048,6 +2975,13 @@
       </border>
     </dxf>
     <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor theme="4"/>
@@ -1055,190 +2989,6 @@
         </patternFill>
       </fill>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="double">
-          <color theme="4"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="double">
-          <color theme="4"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="double">
-          <color theme="4"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="double">
-          <color theme="4"/>
-        </bottom>
-      </border>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1374,11 +3124,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="82893568"/>
-        <c:axId val="82894144"/>
+        <c:axId val="84187904"/>
+        <c:axId val="84188480"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="82893568"/>
+        <c:axId val="84187904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -1415,13 +3165,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="82894144"/>
+        <c:crossAx val="84188480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.1"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="82894144"/>
+        <c:axId val="84188480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -1453,7 +3203,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="82893568"/>
+        <c:crossAx val="84187904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.1"/>
@@ -1509,7 +3259,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>0.1875</c:v>
+                  <c:v>0.25</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1521,7 +3271,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>0.875</c:v>
+                  <c:v>0.75</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1586,11 +3336,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="118473856"/>
-        <c:axId val="118474432"/>
+        <c:axId val="122638848"/>
+        <c:axId val="122639424"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="118473856"/>
+        <c:axId val="122638848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -1627,13 +3377,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="118474432"/>
+        <c:crossAx val="122639424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.1"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="118474432"/>
+        <c:axId val="122639424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -1665,7 +3415,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="118473856"/>
+        <c:crossAx val="122638848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.1"/>
@@ -1798,11 +3548,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="67736064"/>
-        <c:axId val="67737216"/>
+        <c:axId val="122641728"/>
+        <c:axId val="81698816"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="67736064"/>
+        <c:axId val="122641728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -1839,13 +3589,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="67737216"/>
+        <c:crossAx val="81698816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.1"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="67737216"/>
+        <c:axId val="81698816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -1877,7 +3627,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="67736064"/>
+        <c:crossAx val="122641728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.1"/>
@@ -2010,11 +3760,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="118477312"/>
-        <c:axId val="118477888"/>
+        <c:axId val="81701696"/>
+        <c:axId val="81702272"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="118477312"/>
+        <c:axId val="81701696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -2051,13 +3801,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="118477888"/>
+        <c:crossAx val="81702272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.1"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="118477888"/>
+        <c:axId val="81702272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -2089,7 +3839,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="118477312"/>
+        <c:crossAx val="81701696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.1"/>
@@ -2222,11 +3972,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="118479616"/>
-        <c:axId val="118480192"/>
+        <c:axId val="81704000"/>
+        <c:axId val="81704576"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="118479616"/>
+        <c:axId val="81704000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -2263,13 +4013,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="118480192"/>
+        <c:crossAx val="81704576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.1"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="118480192"/>
+        <c:axId val="81704576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -2301,7 +4051,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="118479616"/>
+        <c:crossAx val="81704000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.1"/>
@@ -2434,11 +4184,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="125194176"/>
-        <c:axId val="125195328"/>
+        <c:axId val="84189184"/>
+        <c:axId val="84189760"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="125194176"/>
+        <c:axId val="84189184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -2475,13 +4225,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="125195328"/>
+        <c:crossAx val="84189760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.1"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="125195328"/>
+        <c:axId val="84189760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -2513,7 +4263,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="125194176"/>
+        <c:crossAx val="84189184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.1"/>
@@ -2744,38 +4494,44 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:G20" totalsRowShown="0" headerRowDxfId="55">
-  <autoFilter ref="A1:G20"/>
-  <tableColumns count="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:K20" totalsRowShown="0" headerRowDxfId="230">
+  <autoFilter ref="A1:K20"/>
+  <tableColumns count="11">
     <tableColumn id="1" name="Test"/>
     <tableColumn id="2" name="XML Parser"/>
     <tableColumn id="7" name="Test Title"/>
     <tableColumn id="3" name="Test Tag"/>
     <tableColumn id="4" name="Safety in 4.5.1 and lower"/>
-    <tableColumn id="5" name="Safety in 4.5.2 and up" dataDxfId="54"/>
-    <tableColumn id="6" name="Test Description" dataDxfId="53"/>
+    <tableColumn id="8" name="Fortify Detection (.NET 4.5.1)" dataDxfId="116"/>
+    <tableColumn id="9" name="Contrast Detection (4.5.1)" dataDxfId="115"/>
+    <tableColumn id="5" name="Safety in 4.5.2 and up" dataDxfId="229"/>
+    <tableColumn id="10" name="Fortify Detection (4.5.2)" dataDxfId="118"/>
+    <tableColumn id="11" name="Contrast Detection (4.5.2)" dataDxfId="117"/>
+    <tableColumn id="6" name="Test Description" dataDxfId="228"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A1:F12" totalsRowShown="0" headerRowDxfId="24" headerRowBorderDxfId="22" tableBorderDxfId="23" totalsRowBorderDxfId="21" headerRowCellStyle="Warning Text" dataCellStyle="Warning Text">
-  <autoFilter ref="A1:F12"/>
-  <tableColumns count="6">
-    <tableColumn id="1" name="Test" dataDxfId="20"/>
-    <tableColumn id="2" name="Query Type" dataDxfId="19"/>
-    <tableColumn id="3" name="Test Title" dataDxfId="18"/>
-    <tableColumn id="4" name="Test Tag" dataDxfId="17"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A1:H12" totalsRowShown="0" headerRowDxfId="227" headerRowBorderDxfId="226" tableBorderDxfId="225" totalsRowBorderDxfId="224">
+  <autoFilter ref="A1:H12"/>
+  <tableColumns count="8">
+    <tableColumn id="1" name="Test" dataDxfId="223"/>
+    <tableColumn id="2" name="Query Type" dataDxfId="222"/>
+    <tableColumn id="3" name="Test Title" dataDxfId="221"/>
+    <tableColumn id="4" name="Test Tag" dataDxfId="220"/>
     <tableColumn id="5" name="Safety"/>
-    <tableColumn id="7" name="Test Description" dataDxfId="16"/>
+    <tableColumn id="6" name="Fortify Detection"/>
+    <tableColumn id="8" name="Contrast Detection"/>
+    <tableColumn id="7" name="Test Description" dataDxfId="219"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A2:I11" totalsRowShown="0" tableBorderDxfId="52">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A2:I11" totalsRowShown="0" tableBorderDxfId="218">
   <autoFilter ref="A2:I11"/>
   <tableColumns count="9">
     <tableColumn id="1" name="XML Parser"/>
@@ -2784,16 +4540,16 @@
     <tableColumn id="4" name="True Negative"/>
     <tableColumn id="5" name="False Positive"/>
     <tableColumn id="6" name="Total"/>
-    <tableColumn id="7" name="True Posistive Rate" dataDxfId="51"/>
-    <tableColumn id="8" name="False Positive Rate" dataDxfId="50"/>
-    <tableColumn id="9" name="Score" dataDxfId="49"/>
+    <tableColumn id="7" name="True Posistive Rate" dataDxfId="217"/>
+    <tableColumn id="8" name="False Positive Rate" dataDxfId="216"/>
+    <tableColumn id="9" name="Score" dataDxfId="215"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table27" displayName="Table27" ref="A30:I39" totalsRowShown="0" tableBorderDxfId="48">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table27" displayName="Table27" ref="A30:I39" totalsRowShown="0" tableBorderDxfId="214">
   <autoFilter ref="A30:I39"/>
   <tableColumns count="9">
     <tableColumn id="1" name="XML Parser"/>
@@ -2802,16 +4558,16 @@
     <tableColumn id="4" name="True Negative"/>
     <tableColumn id="5" name="False Positive"/>
     <tableColumn id="6" name="Total"/>
-    <tableColumn id="7" name="True Posistive Rate" dataDxfId="47"/>
-    <tableColumn id="8" name="False Positive Rate" dataDxfId="46"/>
-    <tableColumn id="9" name="Score" dataDxfId="45"/>
+    <tableColumn id="7" name="True Posistive Rate" dataDxfId="213"/>
+    <tableColumn id="8" name="False Positive Rate" dataDxfId="212"/>
+    <tableColumn id="9" name="Score" dataDxfId="211"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table26" displayName="Table26" ref="A2:I5" totalsRowShown="0" tableBorderDxfId="15">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table26" displayName="Table26" ref="A2:I5" totalsRowShown="0" tableBorderDxfId="210">
   <autoFilter ref="A2:I5"/>
   <tableColumns count="9">
     <tableColumn id="1" name="Query Type"/>
@@ -2820,16 +4576,16 @@
     <tableColumn id="4" name="True Negative"/>
     <tableColumn id="5" name="False Positive"/>
     <tableColumn id="6" name="Total"/>
-    <tableColumn id="7" name="True Posistive Rate" dataDxfId="14"/>
-    <tableColumn id="8" name="False Positive Rate" dataDxfId="13"/>
-    <tableColumn id="9" name="Score" dataDxfId="12"/>
+    <tableColumn id="7" name="True Posistive Rate" dataDxfId="209"/>
+    <tableColumn id="8" name="False Positive Rate" dataDxfId="208"/>
+    <tableColumn id="9" name="Score" dataDxfId="207"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table28" displayName="Table28" ref="A2:I11" totalsRowShown="0" tableBorderDxfId="44">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table28" displayName="Table28" ref="A2:I11" totalsRowShown="0" tableBorderDxfId="206">
   <autoFilter ref="A2:I11"/>
   <tableColumns count="9">
     <tableColumn id="1" name="XML Parser"/>
@@ -2838,16 +4594,16 @@
     <tableColumn id="4" name="True Negative"/>
     <tableColumn id="5" name="False Positive"/>
     <tableColumn id="6" name="Total"/>
-    <tableColumn id="7" name="True Posistive Rate" dataDxfId="43"/>
-    <tableColumn id="8" name="False Positive Rate" dataDxfId="42"/>
-    <tableColumn id="9" name="Score" dataDxfId="41"/>
+    <tableColumn id="7" name="True Posistive Rate" dataDxfId="205"/>
+    <tableColumn id="8" name="False Positive Rate" dataDxfId="204"/>
+    <tableColumn id="9" name="Score" dataDxfId="203"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table279" displayName="Table279" ref="A30:I39" totalsRowShown="0" tableBorderDxfId="40">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table279" displayName="Table279" ref="A30:I39" totalsRowShown="0" tableBorderDxfId="202">
   <autoFilter ref="A30:I39"/>
   <tableColumns count="9">
     <tableColumn id="1" name="XML Parser"/>
@@ -2856,16 +4612,16 @@
     <tableColumn id="4" name="True Negative"/>
     <tableColumn id="5" name="False Positive"/>
     <tableColumn id="6" name="Total"/>
-    <tableColumn id="7" name="True Posistive Rate" dataDxfId="39"/>
-    <tableColumn id="8" name="False Positive Rate" dataDxfId="38"/>
-    <tableColumn id="9" name="Score" dataDxfId="37"/>
+    <tableColumn id="7" name="True Posistive Rate" dataDxfId="201"/>
+    <tableColumn id="8" name="False Positive Rate" dataDxfId="200"/>
+    <tableColumn id="9" name="Score" dataDxfId="199"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Table2610" displayName="Table2610" ref="A2:I5" totalsRowShown="0" tableBorderDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Table2610" displayName="Table2610" ref="A2:I5" totalsRowShown="0" tableBorderDxfId="198">
   <autoFilter ref="A2:I5"/>
   <tableColumns count="9">
     <tableColumn id="1" name="Query Type"/>
@@ -2874,9 +4630,9 @@
     <tableColumn id="4" name="True Negative"/>
     <tableColumn id="5" name="False Positive"/>
     <tableColumn id="6" name="Total"/>
-    <tableColumn id="7" name="True Posistive Rate" dataDxfId="2"/>
-    <tableColumn id="8" name="False Positive Rate" dataDxfId="1"/>
-    <tableColumn id="9" name="Score" dataDxfId="0"/>
+    <tableColumn id="7" name="True Posistive Rate" dataDxfId="197"/>
+    <tableColumn id="8" name="False Positive Rate" dataDxfId="196"/>
+    <tableColumn id="9" name="Score" dataDxfId="195"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3172,11 +4928,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G39"/>
+  <dimension ref="A1:K39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B22" sqref="B22"/>
+      <selection pane="bottomLeft" activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3186,11 +4942,14 @@
     <col min="3" max="3" width="61.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="28.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="117.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="114.28515625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>78</v>
       </c>
@@ -3207,13 +4966,25 @@
         <v>5</v>
       </c>
       <c r="F1" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="H1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -3229,14 +5000,26 @@
       <c r="E2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="G2" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="I2" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="J2" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="K2" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -3252,14 +5035,26 @@
       <c r="E3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="G3" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="H3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="I3" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="J3" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="K3" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -3275,14 +5070,26 @@
       <c r="E4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="F4" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="G4" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="H4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="I4" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="J4" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="K4" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -3298,14 +5105,26 @@
       <c r="E5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="F5" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="G5" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="H5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="I5" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="J5" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="K5" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -3321,14 +5140,26 @@
       <c r="E6" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="F6" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="G6" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="H6" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="I6" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="J6" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="K6" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -3345,13 +5176,25 @@
         <v>2</v>
       </c>
       <c r="F7" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="G7" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="H7" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="G7" s="1" t="s">
+      <c r="I7" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="J7" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="K7" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -3368,13 +5211,25 @@
         <v>3</v>
       </c>
       <c r="F8" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="G8" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="H8" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="G8" s="1" t="s">
+      <c r="I8" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="J8" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="K8" s="1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -3390,14 +5245,26 @@
       <c r="E9" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="F9" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="G9" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="H9" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="G9" s="1" t="s">
+      <c r="I9" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="J9" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="K9" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -3413,14 +5280,26 @@
       <c r="E10" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F10" s="2" t="s">
+      <c r="F10" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="G10" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="H10" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G10" s="1" t="s">
+      <c r="I10" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="J10" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="K10" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -3436,14 +5315,26 @@
       <c r="E11" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F11" s="2" t="s">
+      <c r="F11" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="G11" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="H11" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="G11" s="1" t="s">
+      <c r="I11" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="J11" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="K11" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -3459,14 +5350,26 @@
       <c r="E12" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F12" s="2" t="s">
+      <c r="F12" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="G12" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="H12" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G12" s="1" t="s">
+      <c r="I12" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="J12" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="K12" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -3482,14 +5385,26 @@
       <c r="E13" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F13" s="2" t="s">
+      <c r="F13" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="G13" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="H13" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G13" s="1" t="s">
+      <c r="I13" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="J13" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="K13" s="1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -3506,13 +5421,25 @@
         <v>2</v>
       </c>
       <c r="F14" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="G14" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="H14" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="G14" s="1" t="s">
+      <c r="I14" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="J14" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="K14" s="1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>14</v>
       </c>
@@ -3529,13 +5456,25 @@
         <v>3</v>
       </c>
       <c r="F15" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="G15" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="H15" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="G15" s="1" t="s">
+      <c r="I15" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="J15" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="K15" s="1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>15</v>
       </c>
@@ -3551,14 +5490,26 @@
       <c r="E16" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F16" s="2" t="s">
+      <c r="F16" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="G16" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="H16" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="G16" s="1" t="s">
+      <c r="I16" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="J16" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="K16" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>16</v>
       </c>
@@ -3575,13 +5526,25 @@
         <v>2</v>
       </c>
       <c r="F17" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="G17" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="H17" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="G17" s="1" t="s">
+      <c r="I17" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="J17" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="K17" s="1" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>17</v>
       </c>
@@ -3598,13 +5561,25 @@
         <v>3</v>
       </c>
       <c r="F18" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="G18" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="H18" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="G18" s="1" t="s">
+      <c r="I18" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="J18" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="K18" s="1" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>18</v>
       </c>
@@ -3621,13 +5596,25 @@
         <v>3</v>
       </c>
       <c r="F19" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="G19" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="H19" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="G19" s="1" t="s">
+      <c r="I19" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="J19" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="K19" s="1" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>19</v>
       </c>
@@ -3643,83 +5630,101 @@
       <c r="E20" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F20" s="2" t="s">
+      <c r="F20" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="G20" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="H20" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="G20" s="1" t="s">
+      <c r="I20" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="J20" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="K20" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
       <c r="B21" s="3"/>
       <c r="C21" s="2"/>
       <c r="E21" s="4"/>
       <c r="F21" s="6"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G21" s="6"/>
+      <c r="H21" s="6"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
       <c r="B22" s="3"/>
       <c r="C22" s="2"/>
       <c r="E22" s="4"/>
       <c r="F22" s="6"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G22" s="6"/>
+      <c r="H22" s="6"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
       <c r="B23" s="3"/>
       <c r="C23" s="2"/>
       <c r="E23" s="4"/>
       <c r="F23" s="6"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G23" s="6"/>
+      <c r="H23" s="6"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
       <c r="B24" s="3"/>
       <c r="C24" s="2"/>
       <c r="E24" s="2"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
       <c r="B25" s="3"/>
       <c r="C25" s="2"/>
       <c r="E25" s="2"/>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
       <c r="B26" s="3"/>
       <c r="C26" s="2"/>
       <c r="E26" s="2"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
       <c r="B27" s="3"/>
       <c r="C27" s="2"/>
       <c r="E27" s="2"/>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
       <c r="B28" s="3"/>
       <c r="C28" s="2"/>
       <c r="E28" s="2"/>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="2"/>
       <c r="B29" s="3"/>
       <c r="C29" s="2"/>
       <c r="E29" s="2"/>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="2"/>
       <c r="B30" s="3"/>
       <c r="C30" s="2"/>
       <c r="E30" s="2"/>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="2"/>
       <c r="B31" s="3"/>
       <c r="C31" s="2"/>
       <c r="E31" s="2"/>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="2"/>
       <c r="B32" s="3"/>
       <c r="C32" s="2"/>
@@ -3768,20 +5773,28 @@
       <c r="E39" s="2"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="F2:F6 F9:F10 E11:F13 F16 E2:E20 F20">
-    <cfRule type="containsText" dxfId="11" priority="3" operator="containsText" text="Safe">
+  <conditionalFormatting sqref="E2:E20 F20:J20 F16:J16 G7:G20 J2:J20 I18:I19 I15:I16 F9:J13 I8:I11 F2:J6">
+    <cfRule type="containsText" dxfId="114" priority="5" operator="containsText" text="Safe">
       <formula>NOT(ISERROR(SEARCH("Safe",E2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="4" operator="containsText" text="Safe">
+    <cfRule type="containsText" dxfId="113" priority="6" operator="containsText" text="Safe">
       <formula>NOT(ISERROR(SEARCH("Safe",E2)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:F20">
-    <cfRule type="containsText" dxfId="9" priority="1" operator="containsText" text="Unsafe">
+  <conditionalFormatting sqref="E2:J20">
+    <cfRule type="containsText" dxfId="112" priority="3" operator="containsText" text="Unsafe">
       <formula>NOT(ISERROR(SEARCH("Unsafe",E2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="2" operator="containsText" text="Safe">
+    <cfRule type="containsText" dxfId="111" priority="4" operator="containsText" text="Safe">
       <formula>NOT(ISERROR(SEARCH("Safe",E2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F1:G1048576 I1:J20">
+    <cfRule type="containsText" dxfId="110" priority="1" operator="containsText" text="Fail">
+      <formula>NOT(ISERROR(SEARCH("Fail",F1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="109" priority="2" operator="containsText" text="Pass">
+      <formula>NOT(ISERROR(SEARCH("Pass",F1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3794,10 +5807,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3807,277 +5820,363 @@
     <col min="3" max="3" width="84.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="171.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="114.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="171.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="25" t="s">
+    <row r="1" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="22" t="s">
         <v>78</v>
       </c>
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="22" t="s">
         <v>77</v>
       </c>
-      <c r="C1" s="25" t="s">
+      <c r="C1" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="D1" s="25" t="s">
+      <c r="D1" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="25" t="s">
+      <c r="E1" s="22" t="s">
         <v>81</v>
       </c>
-      <c r="F1" s="26" t="s">
+      <c r="F1" s="22" t="s">
+        <v>117</v>
+      </c>
+      <c r="G1" s="22" t="s">
+        <v>118</v>
+      </c>
+      <c r="H1" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="11"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="19">
+      <c r="I1" s="11"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="16">
         <v>1</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="16" t="s">
         <v>79</v>
       </c>
-      <c r="C2" s="19" t="s">
+      <c r="C2" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="D2" s="19" t="s">
+      <c r="D2" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="E2" s="19" t="s">
+      <c r="E2" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="23" t="s">
+      <c r="F2" s="17" t="s">
+        <v>120</v>
+      </c>
+      <c r="G2" s="17" t="s">
+        <v>120</v>
+      </c>
+      <c r="H2" s="20" t="s">
         <v>92</v>
       </c>
-      <c r="G2" s="11"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="20">
+      <c r="I2" s="11"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="17">
         <v>2</v>
       </c>
-      <c r="B3" s="20" t="s">
+      <c r="B3" s="17" t="s">
         <v>79</v>
       </c>
-      <c r="C3" s="20" t="s">
+      <c r="C3" s="17" t="s">
         <v>83</v>
       </c>
-      <c r="D3" s="20" t="s">
+      <c r="D3" s="17" t="s">
         <v>86</v>
       </c>
-      <c r="E3" s="19" t="s">
+      <c r="E3" s="16" t="s">
         <v>2</v>
       </c>
       <c r="F3" s="24" t="s">
+        <v>121</v>
+      </c>
+      <c r="G3" s="24" t="s">
+        <v>120</v>
+      </c>
+      <c r="H3" s="21" t="s">
         <v>91</v>
       </c>
-      <c r="G3" s="11"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="19">
+      <c r="I3" s="11"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="16">
         <v>3</v>
       </c>
-      <c r="B4" s="19" t="s">
+      <c r="B4" s="16" t="s">
         <v>79</v>
       </c>
-      <c r="C4" s="19" t="s">
+      <c r="C4" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="D4" s="19" t="s">
+      <c r="D4" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="E4" s="19" t="s">
+      <c r="E4" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="23" t="s">
+      <c r="F4" s="24" t="s">
+        <v>121</v>
+      </c>
+      <c r="G4" s="17" t="s">
+        <v>121</v>
+      </c>
+      <c r="H4" s="20" t="s">
         <v>93</v>
       </c>
-      <c r="G4" s="11"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="20">
+      <c r="I4" s="11"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="17">
         <v>4</v>
       </c>
-      <c r="B5" s="20" t="s">
+      <c r="B5" s="17" t="s">
         <v>79</v>
       </c>
-      <c r="C5" s="20" t="s">
+      <c r="C5" s="17" t="s">
         <v>89</v>
       </c>
-      <c r="D5" s="20" t="s">
+      <c r="D5" s="17" t="s">
         <v>88</v>
       </c>
-      <c r="E5" s="19" t="s">
+      <c r="E5" s="16" t="s">
         <v>2</v>
       </c>
       <c r="F5" s="24" t="s">
+        <v>121</v>
+      </c>
+      <c r="G5" s="17" t="s">
+        <v>121</v>
+      </c>
+      <c r="H5" s="21" t="s">
         <v>94</v>
       </c>
-      <c r="G5" s="11"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="19">
+      <c r="I5" s="11"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="16">
         <v>5</v>
       </c>
-      <c r="B6" s="19" t="s">
+      <c r="B6" s="16" t="s">
         <v>79</v>
       </c>
-      <c r="C6" s="19" t="s">
+      <c r="C6" s="16" t="s">
         <v>90</v>
       </c>
-      <c r="D6" s="20" t="s">
+      <c r="D6" s="17" t="s">
         <v>88</v>
       </c>
-      <c r="E6" s="19" t="s">
+      <c r="E6" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="F6" s="23" t="s">
+      <c r="F6" s="24" t="s">
+        <v>121</v>
+      </c>
+      <c r="G6" s="17" t="s">
+        <v>121</v>
+      </c>
+      <c r="H6" s="20" t="s">
         <v>95</v>
       </c>
-      <c r="G6" s="11"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="20">
+      <c r="I6" s="11"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="17">
         <v>6</v>
       </c>
-      <c r="B7" s="20" t="s">
+      <c r="B7" s="17" t="s">
         <v>79</v>
       </c>
-      <c r="C7" s="21" t="s">
+      <c r="C7" s="18" t="s">
         <v>96</v>
       </c>
-      <c r="D7" s="20" t="s">
+      <c r="D7" s="17" t="s">
         <v>98</v>
       </c>
-      <c r="E7" s="22" t="s">
+      <c r="E7" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="F7" s="24" t="s">
+      <c r="F7" s="17" t="s">
+        <v>120</v>
+      </c>
+      <c r="G7" s="17" t="s">
+        <v>120</v>
+      </c>
+      <c r="H7" s="21" t="s">
         <v>106</v>
       </c>
-      <c r="G7" s="11"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="19">
+      <c r="I7" s="11"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="16">
         <v>7</v>
       </c>
-      <c r="B8" s="19" t="s">
+      <c r="B8" s="16" t="s">
         <v>79</v>
       </c>
-      <c r="C8" s="19" t="s">
+      <c r="C8" s="16" t="s">
         <v>97</v>
       </c>
-      <c r="D8" s="19" t="s">
+      <c r="D8" s="16" t="s">
         <v>99</v>
       </c>
-      <c r="E8" s="22" t="s">
+      <c r="E8" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="F8" s="24" t="s">
+      <c r="F8" s="17" t="s">
+        <v>120</v>
+      </c>
+      <c r="G8" s="17" t="s">
+        <v>120</v>
+      </c>
+      <c r="H8" s="21" t="s">
         <v>105</v>
       </c>
-      <c r="G8" s="11"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="32">
+      <c r="I8" s="11"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="29">
         <v>8</v>
       </c>
-      <c r="B9" s="29" t="s">
+      <c r="B9" s="26" t="s">
         <v>80</v>
       </c>
-      <c r="C9" s="29" t="s">
+      <c r="C9" s="26" t="s">
         <v>101</v>
       </c>
-      <c r="D9" s="29" t="s">
+      <c r="D9" s="26" t="s">
         <v>100</v>
       </c>
-      <c r="E9" s="30" t="s">
+      <c r="E9" s="27" t="s">
+        <v>119</v>
+      </c>
+      <c r="F9" s="35" t="s">
+        <v>119</v>
+      </c>
+      <c r="G9" s="35" t="s">
+        <v>119</v>
+      </c>
+      <c r="H9" s="28" t="s">
+        <v>107</v>
+      </c>
+      <c r="I9" s="11"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="16">
+        <v>9</v>
+      </c>
+      <c r="B10" s="17" t="s">
+        <v>80</v>
+      </c>
+      <c r="C10" s="16" t="s">
+        <v>102</v>
+      </c>
+      <c r="D10" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="E10" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="F10" s="17" t="s">
+        <v>121</v>
+      </c>
+      <c r="G10" s="17" t="s">
+        <v>121</v>
+      </c>
+      <c r="H10" s="20" t="s">
+        <v>104</v>
+      </c>
+      <c r="I10" s="11"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="17">
+        <v>10</v>
+      </c>
+      <c r="B11" s="17" t="s">
+        <v>80</v>
+      </c>
+      <c r="C11" s="17" t="s">
+        <v>108</v>
+      </c>
+      <c r="D11" s="17" t="s">
+        <v>113</v>
+      </c>
+      <c r="E11" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="F11" s="17" t="s">
+        <v>121</v>
+      </c>
+      <c r="G11" s="17" t="s">
+        <v>121</v>
+      </c>
+      <c r="H11" s="30" t="s">
+        <v>109</v>
+      </c>
+      <c r="I11" s="11"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="24">
+        <v>11</v>
+      </c>
+      <c r="B12" s="17" t="s">
+        <v>80</v>
+      </c>
+      <c r="C12" s="24" t="s">
+        <v>111</v>
+      </c>
+      <c r="D12" s="24" t="s">
+        <v>112</v>
+      </c>
+      <c r="E12" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="F9" s="31" t="s">
-        <v>107</v>
-      </c>
-      <c r="G9" s="11"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="19">
-        <v>9</v>
-      </c>
-      <c r="B10" s="20" t="s">
-        <v>80</v>
-      </c>
-      <c r="C10" s="19" t="s">
-        <v>102</v>
-      </c>
-      <c r="D10" s="19" t="s">
-        <v>103</v>
-      </c>
-      <c r="E10" s="20" t="s">
-        <v>2</v>
-      </c>
-      <c r="F10" s="23" t="s">
-        <v>104</v>
-      </c>
-      <c r="G10" s="11"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="20">
-        <v>10</v>
-      </c>
-      <c r="B11" s="20" t="s">
-        <v>80</v>
-      </c>
-      <c r="C11" s="20" t="s">
-        <v>108</v>
-      </c>
-      <c r="D11" s="20" t="s">
-        <v>113</v>
-      </c>
-      <c r="E11" s="20" t="s">
-        <v>2</v>
-      </c>
-      <c r="F11" s="33" t="s">
-        <v>109</v>
-      </c>
-      <c r="G11" s="11"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="27">
-        <v>11</v>
-      </c>
-      <c r="B12" s="20" t="s">
-        <v>80</v>
-      </c>
-      <c r="C12" s="27" t="s">
-        <v>111</v>
-      </c>
-      <c r="D12" s="27" t="s">
-        <v>112</v>
-      </c>
-      <c r="E12" s="27" t="s">
-        <v>3</v>
-      </c>
-      <c r="F12" s="28" t="s">
+      <c r="F12" s="24" t="s">
+        <v>120</v>
+      </c>
+      <c r="G12" s="24" t="s">
+        <v>120</v>
+      </c>
+      <c r="H12" s="25" t="s">
         <v>110</v>
       </c>
-      <c r="G12" s="11"/>
+      <c r="I12" s="11"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="E2:E12">
-    <cfRule type="containsText" dxfId="7" priority="1" operator="containsText" text="Unsafe">
+  <conditionalFormatting sqref="E2:G12">
+    <cfRule type="containsText" dxfId="108" priority="4" operator="containsText" text="Unsafe">
       <formula>NOT(ISERROR(SEARCH("Unsafe",E2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="2" operator="containsText" text="Safe">
+    <cfRule type="containsText" dxfId="107" priority="5" operator="containsText" text="Safe">
       <formula>NOT(ISERROR(SEARCH("Safe",E2)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E12">
-    <cfRule type="containsText" dxfId="5" priority="3" operator="containsText" text="Safe">
+  <conditionalFormatting sqref="E2:G12">
+    <cfRule type="containsText" dxfId="106" priority="6" operator="containsText" text="Safe">
       <formula>NOT(ISERROR(SEARCH("Safe",E2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="4" operator="containsText" text="Safe">
+    <cfRule type="containsText" dxfId="105" priority="7" operator="containsText" text="Safe">
       <formula>NOT(ISERROR(SEARCH("Safe",E2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F1:F1048576 G2">
+    <cfRule type="containsText" dxfId="104" priority="3" operator="containsText" text="Pass">
+      <formula>NOT(ISERROR(SEARCH("Pass",F1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F1:G1048576">
+    <cfRule type="containsText" dxfId="103" priority="1" operator="containsText" text="Fail">
+      <formula>NOT(ISERROR(SEARCH("Fail",F1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="102" priority="2" operator="containsText" text="Pass">
+      <formula>NOT(ISERROR(SEARCH("Pass",F1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4092,7 +6191,7 @@
   <dimension ref="A1:K55"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4110,17 +6209,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="31" t="s">
         <v>73</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
@@ -4150,7 +6249,7 @@
       <c r="I2" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="K2" s="17" t="s">
+      <c r="K2" s="32" t="s">
         <v>75</v>
       </c>
     </row>
@@ -4182,7 +6281,7 @@
         <f>(Table2[[#This Row],[True Posistive Rate]]+(1 - Table2[[#This Row],[False Positive Rate]])) - 1</f>
         <v>1</v>
       </c>
-      <c r="K3" s="18"/>
+      <c r="K3" s="33"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
@@ -4212,7 +6311,7 @@
         <f>(Table2[[#This Row],[True Posistive Rate]]+(1 - Table2[[#This Row],[False Positive Rate]])) - 1</f>
         <v>1</v>
       </c>
-      <c r="K4" s="18"/>
+      <c r="K4" s="33"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
@@ -4242,7 +6341,7 @@
         <f>(Table2[[#This Row],[True Posistive Rate]]+(1 - Table2[[#This Row],[False Positive Rate]])) - 1</f>
         <v>1</v>
       </c>
-      <c r="K5" s="18"/>
+      <c r="K5" s="33"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
@@ -4272,7 +6371,7 @@
         <f>(Table2[[#This Row],[True Posistive Rate]]+(1 - Table2[[#This Row],[False Positive Rate]])) - 1</f>
         <v>1</v>
       </c>
-      <c r="K6" s="18"/>
+      <c r="K6" s="33"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
@@ -4302,7 +6401,7 @@
         <f>(Table2[[#This Row],[True Posistive Rate]]+(1 - Table2[[#This Row],[False Positive Rate]])) - 1</f>
         <v>1</v>
       </c>
-      <c r="K7" s="18"/>
+      <c r="K7" s="33"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
@@ -4332,7 +6431,7 @@
         <f>(Table2[[#This Row],[True Posistive Rate]]+(1 - Table2[[#This Row],[False Positive Rate]])) - 1</f>
         <v>1</v>
       </c>
-      <c r="K8" s="18"/>
+      <c r="K8" s="33"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
@@ -4362,7 +6461,7 @@
         <f>(Table2[[#This Row],[True Posistive Rate]]+(1 - Table2[[#This Row],[False Positive Rate]])) - 1</f>
         <v>1</v>
       </c>
-      <c r="K9" s="18"/>
+      <c r="K9" s="33"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
@@ -4392,7 +6491,7 @@
         <f>(Table2[[#This Row],[True Posistive Rate]]+(1 - Table2[[#This Row],[False Positive Rate]])) - 1</f>
         <v>0</v>
       </c>
-      <c r="K10" s="18"/>
+      <c r="K10" s="33"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
@@ -4430,7 +6529,7 @@
         <f>ROUND(AVERAGE(I3:I10)*100, 0)</f>
         <v>88</v>
       </c>
-      <c r="K11" s="18"/>
+      <c r="K11" s="33"/>
     </row>
     <row r="12" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="11"/>
@@ -4600,17 +6699,17 @@
       <c r="I27" s="10"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="16" t="s">
+      <c r="A29" s="31" t="s">
         <v>74</v>
       </c>
-      <c r="B29" s="16"/>
-      <c r="C29" s="16"/>
-      <c r="D29" s="16"/>
-      <c r="E29" s="16"/>
-      <c r="F29" s="16"/>
-      <c r="G29" s="16"/>
-      <c r="H29" s="16"/>
-      <c r="I29" s="16"/>
+      <c r="B29" s="31"/>
+      <c r="C29" s="31"/>
+      <c r="D29" s="31"/>
+      <c r="E29" s="31"/>
+      <c r="F29" s="31"/>
+      <c r="G29" s="31"/>
+      <c r="H29" s="31"/>
+      <c r="I29" s="31"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="11" t="s">
@@ -4823,29 +6922,29 @@
       <c r="A37" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="B37" s="11">
-        <v>1</v>
-      </c>
+      <c r="B37" s="11"/>
       <c r="C37" s="11"/>
       <c r="D37" s="11">
         <v>1</v>
       </c>
-      <c r="E37" s="11"/>
+      <c r="E37" s="11">
+        <v>1</v>
+      </c>
       <c r="F37" s="11">
         <f>SUM(Table27[[#This Row],[True Positive]:[False Positive]])</f>
         <v>2</v>
       </c>
       <c r="G37" s="13">
         <f>IF(Table27[[#This Row],[True Positive]]+Table27[[#This Row],[False Negative]]=0,0,Table27[[#This Row],[True Positive]]/(Table27[[#This Row],[True Positive]]+Table27[[#This Row],[False Negative]]))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H37" s="13">
         <f>Table27[[#This Row],[False Positive]]/(Table27[[#This Row],[False Positive]]+Table27[[#This Row],[True Negative]])</f>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="I37" s="13">
         <f>(Table27[[#This Row],[True Posistive Rate]]+(1 - Table27[[#This Row],[False Positive Rate]])) - 1</f>
-        <v>1</v>
+        <v>-0.5</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
@@ -4883,7 +6982,7 @@
       </c>
       <c r="B39" s="9">
         <f>SUM(B31:B38)</f>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C39" s="9">
         <f t="shared" ref="C39:F39" si="0">SUM(C31:C38)</f>
@@ -4895,7 +6994,7 @@
       </c>
       <c r="E39" s="9">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F39" s="9">
         <f t="shared" si="0"/>
@@ -4903,15 +7002,15 @@
       </c>
       <c r="G39" s="9">
         <f>AVERAGE(G31:G38)</f>
-        <v>0.875</v>
+        <v>0.75</v>
       </c>
       <c r="H39" s="9">
         <f>AVERAGE(H31:H38)</f>
-        <v>0.1875</v>
+        <v>0.25</v>
       </c>
       <c r="I39" s="9">
         <f>ROUND(AVERAGE(I31:I38)*100, 0)</f>
-        <v>69</v>
+        <v>50</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
@@ -5169,7 +7268,7 @@
         <v>72</v>
       </c>
       <c r="J2" s="11"/>
-      <c r="K2" s="17" t="s">
+      <c r="K2" s="32" t="s">
         <v>114</v>
       </c>
     </row>
@@ -5202,7 +7301,7 @@
         <v>0</v>
       </c>
       <c r="J3" s="11"/>
-      <c r="K3" s="18"/>
+      <c r="K3" s="33"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
@@ -5233,7 +7332,7 @@
         <v>0</v>
       </c>
       <c r="J4" s="11"/>
-      <c r="K4" s="18"/>
+      <c r="K4" s="33"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
@@ -5272,7 +7371,7 @@
         <v>0</v>
       </c>
       <c r="J5" s="11"/>
-      <c r="K5" s="18"/>
+      <c r="K5" s="33"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="11"/>
@@ -5285,7 +7384,7 @@
       <c r="H6" s="11"/>
       <c r="I6" s="11"/>
       <c r="J6" s="11"/>
-      <c r="K6" s="18"/>
+      <c r="K6" s="33"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="11"/>
@@ -5298,7 +7397,7 @@
       <c r="H7" s="11"/>
       <c r="I7" s="11"/>
       <c r="J7" s="11"/>
-      <c r="K7" s="18"/>
+      <c r="K7" s="33"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="11"/>
@@ -5311,7 +7410,7 @@
       <c r="H8" s="11"/>
       <c r="I8" s="11"/>
       <c r="J8" s="11"/>
-      <c r="K8" s="18"/>
+      <c r="K8" s="33"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="11"/>
@@ -5324,7 +7423,7 @@
       <c r="H9" s="11"/>
       <c r="I9" s="11"/>
       <c r="J9" s="11"/>
-      <c r="K9" s="18"/>
+      <c r="K9" s="33"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="11"/>
@@ -5337,7 +7436,7 @@
       <c r="H10" s="11"/>
       <c r="I10" s="11"/>
       <c r="J10" s="11"/>
-      <c r="K10" s="18"/>
+      <c r="K10" s="33"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="11"/>
@@ -5350,7 +7449,7 @@
       <c r="H11" s="11"/>
       <c r="I11" s="11"/>
       <c r="J11" s="11"/>
-      <c r="K11" s="18"/>
+      <c r="K11" s="33"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="11"/>
@@ -5555,17 +7654,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="31" t="s">
         <v>73</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
       <c r="J1" s="11"/>
       <c r="K1" s="11"/>
     </row>
@@ -5598,7 +7697,7 @@
         <v>72</v>
       </c>
       <c r="J2" s="11"/>
-      <c r="K2" s="17" t="s">
+      <c r="K2" s="32" t="s">
         <v>76</v>
       </c>
     </row>
@@ -5631,7 +7730,7 @@
         <v>0</v>
       </c>
       <c r="J3" s="11"/>
-      <c r="K3" s="18"/>
+      <c r="K3" s="33"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
@@ -5662,7 +7761,7 @@
         <v>0</v>
       </c>
       <c r="J4" s="11"/>
-      <c r="K4" s="18"/>
+      <c r="K4" s="33"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
@@ -5693,7 +7792,7 @@
         <v>0</v>
       </c>
       <c r="J5" s="11"/>
-      <c r="K5" s="18"/>
+      <c r="K5" s="33"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
@@ -5722,7 +7821,7 @@
         <v>0</v>
       </c>
       <c r="J6" s="11"/>
-      <c r="K6" s="18"/>
+      <c r="K6" s="33"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
@@ -5753,7 +7852,7 @@
         <v>0</v>
       </c>
       <c r="J7" s="11"/>
-      <c r="K7" s="18"/>
+      <c r="K7" s="33"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
@@ -5784,7 +7883,7 @@
         <v>0</v>
       </c>
       <c r="J8" s="11"/>
-      <c r="K8" s="18"/>
+      <c r="K8" s="33"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
@@ -5815,7 +7914,7 @@
         <v>0</v>
       </c>
       <c r="J9" s="11"/>
-      <c r="K9" s="18"/>
+      <c r="K9" s="33"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
@@ -5846,7 +7945,7 @@
         <v>0</v>
       </c>
       <c r="J10" s="11"/>
-      <c r="K10" s="18"/>
+      <c r="K10" s="33"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
@@ -5885,7 +7984,7 @@
         <v>0</v>
       </c>
       <c r="J11" s="11"/>
-      <c r="K11" s="18"/>
+      <c r="K11" s="33"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="11"/>
@@ -6109,17 +8208,17 @@
       <c r="K28" s="11"/>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="16" t="s">
+      <c r="A29" s="31" t="s">
         <v>74</v>
       </c>
-      <c r="B29" s="16"/>
-      <c r="C29" s="16"/>
-      <c r="D29" s="16"/>
-      <c r="E29" s="16"/>
-      <c r="F29" s="16"/>
-      <c r="G29" s="16"/>
-      <c r="H29" s="16"/>
-      <c r="I29" s="16"/>
+      <c r="B29" s="31"/>
+      <c r="C29" s="31"/>
+      <c r="D29" s="31"/>
+      <c r="E29" s="31"/>
+      <c r="F29" s="31"/>
+      <c r="G29" s="31"/>
+      <c r="H29" s="31"/>
+      <c r="I29" s="31"/>
       <c r="J29" s="11"/>
       <c r="K29" s="11"/>
     </row>
@@ -6725,7 +8824,7 @@
         <v>72</v>
       </c>
       <c r="J2" s="11"/>
-      <c r="K2" s="17"/>
+      <c r="K2" s="32"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
@@ -6758,7 +8857,7 @@
         <v>0.25</v>
       </c>
       <c r="J3" s="11"/>
-      <c r="K3" s="18"/>
+      <c r="K3" s="33"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
@@ -6789,7 +8888,7 @@
         <v>0</v>
       </c>
       <c r="J4" s="11"/>
-      <c r="K4" s="18"/>
+      <c r="K4" s="33"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
@@ -6828,7 +8927,7 @@
         <v>13</v>
       </c>
       <c r="J5" s="11"/>
-      <c r="K5" s="18"/>
+      <c r="K5" s="33"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="11"/>
@@ -6841,7 +8940,7 @@
       <c r="H6" s="11"/>
       <c r="I6" s="11"/>
       <c r="J6" s="11"/>
-      <c r="K6" s="18"/>
+      <c r="K6" s="33"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="11"/>
@@ -6854,7 +8953,7 @@
       <c r="H7" s="11"/>
       <c r="I7" s="11"/>
       <c r="J7" s="11"/>
-      <c r="K7" s="18"/>
+      <c r="K7" s="33"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="11"/>
@@ -6867,7 +8966,7 @@
       <c r="H8" s="11"/>
       <c r="I8" s="11"/>
       <c r="J8" s="11"/>
-      <c r="K8" s="18"/>
+      <c r="K8" s="33"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="11"/>
@@ -6880,7 +8979,7 @@
       <c r="H9" s="11"/>
       <c r="I9" s="11"/>
       <c r="J9" s="11"/>
-      <c r="K9" s="18"/>
+      <c r="K9" s="33"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="11"/>
@@ -6893,7 +8992,7 @@
       <c r="H10" s="11"/>
       <c r="I10" s="11"/>
       <c r="J10" s="11"/>
-      <c r="K10" s="18"/>
+      <c r="K10" s="33"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="11"/>
@@ -6906,7 +9005,7 @@
       <c r="H11" s="11"/>
       <c r="I11" s="11"/>
       <c r="J11" s="11"/>
-      <c r="K11" s="18"/>
+      <c r="K11" s="33"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="11"/>

</xml_diff>

<commit_message>
Update Contrast results for version 3.4.2
</commit_message>
<xml_diff>
--- a/DotNET Tests and Results.xlsx
+++ b/DotNET Tests and Results.xlsx
@@ -737,6 +737,7 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="2" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -749,1936 +750,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="2" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Total" xfId="1" builtinId="25"/>
   </cellStyles>
-  <dxfs count="231">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="53">
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -2991,6 +1069,76 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -2998,6 +1146,78 @@
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -3124,11 +1344,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="84187904"/>
-        <c:axId val="84188480"/>
+        <c:axId val="92801280"/>
+        <c:axId val="92801856"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="84187904"/>
+        <c:axId val="92801280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -3158,20 +1378,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="84188480"/>
+        <c:crossAx val="92801856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.1"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="84188480"/>
+        <c:axId val="92801856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -3196,14 +1415,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="84187904"/>
+        <c:crossAx val="92801280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.1"/>
@@ -3336,11 +1554,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="122638848"/>
-        <c:axId val="122639424"/>
+        <c:axId val="92803584"/>
+        <c:axId val="92804160"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="122638848"/>
+        <c:axId val="92803584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -3370,20 +1588,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="122639424"/>
+        <c:crossAx val="92804160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.1"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="122639424"/>
+        <c:axId val="92804160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -3408,14 +1625,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="122638848"/>
+        <c:crossAx val="92803584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.1"/>
@@ -3548,11 +1764,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="122641728"/>
-        <c:axId val="81698816"/>
+        <c:axId val="92806464"/>
+        <c:axId val="165167104"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="122641728"/>
+        <c:axId val="92806464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -3582,20 +1798,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="81698816"/>
+        <c:crossAx val="165167104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.1"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="81698816"/>
+        <c:axId val="165167104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -3620,14 +1835,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="122641728"/>
+        <c:crossAx val="92806464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.1"/>
@@ -3760,11 +1974,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="81701696"/>
-        <c:axId val="81702272"/>
+        <c:axId val="165169984"/>
+        <c:axId val="165170560"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="81701696"/>
+        <c:axId val="165169984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -3794,20 +2008,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="81702272"/>
+        <c:crossAx val="165170560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.1"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="81702272"/>
+        <c:axId val="165170560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -3832,14 +2045,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="81701696"/>
+        <c:crossAx val="165169984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.1"/>
@@ -3972,11 +2184,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="81704000"/>
-        <c:axId val="81704576"/>
+        <c:axId val="165172288"/>
+        <c:axId val="165172864"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="81704000"/>
+        <c:axId val="165172288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -4006,20 +2218,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="81704576"/>
+        <c:crossAx val="165172864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.1"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="81704576"/>
+        <c:axId val="165172864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -4044,14 +2255,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="81704000"/>
+        <c:crossAx val="165172288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.1"/>
@@ -4184,11 +2394,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="84189184"/>
-        <c:axId val="84189760"/>
+        <c:axId val="165683200"/>
+        <c:axId val="165683776"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="84189184"/>
+        <c:axId val="165683200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -4218,20 +2428,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="84189760"/>
+        <c:crossAx val="165683776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.1"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="84189760"/>
+        <c:axId val="165683776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -4256,14 +2465,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="84189184"/>
+        <c:crossAx val="165683200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.1"/>
@@ -4494,7 +2702,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:K20" totalsRowShown="0" headerRowDxfId="230">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:K20" totalsRowShown="0" headerRowDxfId="46">
   <autoFilter ref="A1:K20"/>
   <tableColumns count="11">
     <tableColumn id="1" name="Test"/>
@@ -4502,36 +2710,36 @@
     <tableColumn id="7" name="Test Title"/>
     <tableColumn id="3" name="Test Tag"/>
     <tableColumn id="4" name="Safety in 4.5.1 and lower"/>
-    <tableColumn id="8" name="Fortify Detection (.NET 4.5.1)" dataDxfId="116"/>
-    <tableColumn id="9" name="Contrast Detection (4.5.1)" dataDxfId="115"/>
-    <tableColumn id="5" name="Safety in 4.5.2 and up" dataDxfId="229"/>
-    <tableColumn id="10" name="Fortify Detection (4.5.2)" dataDxfId="118"/>
-    <tableColumn id="11" name="Contrast Detection (4.5.2)" dataDxfId="117"/>
-    <tableColumn id="6" name="Test Description" dataDxfId="228"/>
+    <tableColumn id="8" name="Fortify Detection (.NET 4.5.1)" dataDxfId="45"/>
+    <tableColumn id="9" name="Contrast Detection (4.5.1)" dataDxfId="44"/>
+    <tableColumn id="5" name="Safety in 4.5.2 and up" dataDxfId="43"/>
+    <tableColumn id="10" name="Fortify Detection (4.5.2)" dataDxfId="42"/>
+    <tableColumn id="11" name="Contrast Detection (4.5.2)" dataDxfId="41"/>
+    <tableColumn id="6" name="Test Description" dataDxfId="40"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A1:H12" totalsRowShown="0" headerRowDxfId="227" headerRowBorderDxfId="226" tableBorderDxfId="225" totalsRowBorderDxfId="224">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A1:H12" totalsRowShown="0" headerRowDxfId="32" headerRowBorderDxfId="31" tableBorderDxfId="30" totalsRowBorderDxfId="29">
   <autoFilter ref="A1:H12"/>
   <tableColumns count="8">
-    <tableColumn id="1" name="Test" dataDxfId="223"/>
-    <tableColumn id="2" name="Query Type" dataDxfId="222"/>
-    <tableColumn id="3" name="Test Title" dataDxfId="221"/>
-    <tableColumn id="4" name="Test Tag" dataDxfId="220"/>
+    <tableColumn id="1" name="Test" dataDxfId="28"/>
+    <tableColumn id="2" name="Query Type" dataDxfId="27"/>
+    <tableColumn id="3" name="Test Title" dataDxfId="26"/>
+    <tableColumn id="4" name="Test Tag" dataDxfId="25"/>
     <tableColumn id="5" name="Safety"/>
     <tableColumn id="6" name="Fortify Detection"/>
     <tableColumn id="8" name="Contrast Detection"/>
-    <tableColumn id="7" name="Test Description" dataDxfId="219"/>
+    <tableColumn id="7" name="Test Description" dataDxfId="24"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A2:I11" totalsRowShown="0" tableBorderDxfId="218">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A2:I11" totalsRowShown="0" tableBorderDxfId="23">
   <autoFilter ref="A2:I11"/>
   <tableColumns count="9">
     <tableColumn id="1" name="XML Parser"/>
@@ -4540,16 +2748,16 @@
     <tableColumn id="4" name="True Negative"/>
     <tableColumn id="5" name="False Positive"/>
     <tableColumn id="6" name="Total"/>
-    <tableColumn id="7" name="True Posistive Rate" dataDxfId="217"/>
-    <tableColumn id="8" name="False Positive Rate" dataDxfId="216"/>
-    <tableColumn id="9" name="Score" dataDxfId="215"/>
+    <tableColumn id="7" name="True Posistive Rate" dataDxfId="22"/>
+    <tableColumn id="8" name="False Positive Rate" dataDxfId="21"/>
+    <tableColumn id="9" name="Score" dataDxfId="20"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table27" displayName="Table27" ref="A30:I39" totalsRowShown="0" tableBorderDxfId="214">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table27" displayName="Table27" ref="A30:I39" totalsRowShown="0" tableBorderDxfId="19">
   <autoFilter ref="A30:I39"/>
   <tableColumns count="9">
     <tableColumn id="1" name="XML Parser"/>
@@ -4558,16 +2766,16 @@
     <tableColumn id="4" name="True Negative"/>
     <tableColumn id="5" name="False Positive"/>
     <tableColumn id="6" name="Total"/>
-    <tableColumn id="7" name="True Posistive Rate" dataDxfId="213"/>
-    <tableColumn id="8" name="False Positive Rate" dataDxfId="212"/>
-    <tableColumn id="9" name="Score" dataDxfId="211"/>
+    <tableColumn id="7" name="True Posistive Rate" dataDxfId="18"/>
+    <tableColumn id="8" name="False Positive Rate" dataDxfId="17"/>
+    <tableColumn id="9" name="Score" dataDxfId="16"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table26" displayName="Table26" ref="A2:I5" totalsRowShown="0" tableBorderDxfId="210">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table26" displayName="Table26" ref="A2:I5" totalsRowShown="0" tableBorderDxfId="15">
   <autoFilter ref="A2:I5"/>
   <tableColumns count="9">
     <tableColumn id="1" name="Query Type"/>
@@ -4576,16 +2784,16 @@
     <tableColumn id="4" name="True Negative"/>
     <tableColumn id="5" name="False Positive"/>
     <tableColumn id="6" name="Total"/>
-    <tableColumn id="7" name="True Posistive Rate" dataDxfId="209"/>
-    <tableColumn id="8" name="False Positive Rate" dataDxfId="208"/>
-    <tableColumn id="9" name="Score" dataDxfId="207"/>
+    <tableColumn id="7" name="True Posistive Rate" dataDxfId="14"/>
+    <tableColumn id="8" name="False Positive Rate" dataDxfId="13"/>
+    <tableColumn id="9" name="Score" dataDxfId="12"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table28" displayName="Table28" ref="A2:I11" totalsRowShown="0" tableBorderDxfId="206">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table28" displayName="Table28" ref="A2:I11" totalsRowShown="0" tableBorderDxfId="11">
   <autoFilter ref="A2:I11"/>
   <tableColumns count="9">
     <tableColumn id="1" name="XML Parser"/>
@@ -4594,16 +2802,16 @@
     <tableColumn id="4" name="True Negative"/>
     <tableColumn id="5" name="False Positive"/>
     <tableColumn id="6" name="Total"/>
-    <tableColumn id="7" name="True Posistive Rate" dataDxfId="205"/>
-    <tableColumn id="8" name="False Positive Rate" dataDxfId="204"/>
-    <tableColumn id="9" name="Score" dataDxfId="203"/>
+    <tableColumn id="7" name="True Posistive Rate" dataDxfId="10"/>
+    <tableColumn id="8" name="False Positive Rate" dataDxfId="9"/>
+    <tableColumn id="9" name="Score" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table279" displayName="Table279" ref="A30:I39" totalsRowShown="0" tableBorderDxfId="202">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table279" displayName="Table279" ref="A30:I39" totalsRowShown="0" tableBorderDxfId="7">
   <autoFilter ref="A30:I39"/>
   <tableColumns count="9">
     <tableColumn id="1" name="XML Parser"/>
@@ -4612,16 +2820,16 @@
     <tableColumn id="4" name="True Negative"/>
     <tableColumn id="5" name="False Positive"/>
     <tableColumn id="6" name="Total"/>
-    <tableColumn id="7" name="True Posistive Rate" dataDxfId="201"/>
-    <tableColumn id="8" name="False Positive Rate" dataDxfId="200"/>
-    <tableColumn id="9" name="Score" dataDxfId="199"/>
+    <tableColumn id="7" name="True Posistive Rate" dataDxfId="6"/>
+    <tableColumn id="8" name="False Positive Rate" dataDxfId="5"/>
+    <tableColumn id="9" name="Score" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Table2610" displayName="Table2610" ref="A2:I5" totalsRowShown="0" tableBorderDxfId="198">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Table2610" displayName="Table2610" ref="A2:I5" totalsRowShown="0" tableBorderDxfId="3">
   <autoFilter ref="A2:I5"/>
   <tableColumns count="9">
     <tableColumn id="1" name="Query Type"/>
@@ -4630,9 +2838,9 @@
     <tableColumn id="4" name="True Negative"/>
     <tableColumn id="5" name="False Positive"/>
     <tableColumn id="6" name="Total"/>
-    <tableColumn id="7" name="True Posistive Rate" dataDxfId="197"/>
-    <tableColumn id="8" name="False Positive Rate" dataDxfId="196"/>
-    <tableColumn id="9" name="Score" dataDxfId="195"/>
+    <tableColumn id="7" name="True Posistive Rate" dataDxfId="2"/>
+    <tableColumn id="8" name="False Positive Rate" dataDxfId="1"/>
+    <tableColumn id="9" name="Score" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4932,7 +3140,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J7" sqref="J7"/>
+      <selection pane="bottomLeft" activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5074,7 +3282,7 @@
         <v>120</v>
       </c>
       <c r="G4" s="11" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>2</v>
@@ -5083,7 +3291,7 @@
         <v>120</v>
       </c>
       <c r="J4" s="11" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="K4" s="1" t="s">
         <v>48</v>
@@ -5144,7 +3352,7 @@
         <v>120</v>
       </c>
       <c r="G6" s="11" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H6" s="2" t="s">
         <v>2</v>
@@ -5153,7 +3361,7 @@
         <v>120</v>
       </c>
       <c r="J6" s="11" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="K6" s="1" t="s">
         <v>50</v>
@@ -5319,7 +3527,7 @@
         <v>120</v>
       </c>
       <c r="G11" s="11" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H11" s="2" t="s">
         <v>2</v>
@@ -5328,7 +3536,7 @@
         <v>120</v>
       </c>
       <c r="J11" s="11" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="K11" s="1" t="s">
         <v>56</v>
@@ -5634,7 +3842,7 @@
         <v>121</v>
       </c>
       <c r="G20" s="11" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H20" s="2" t="s">
         <v>2</v>
@@ -5643,7 +3851,7 @@
         <v>121</v>
       </c>
       <c r="J20" s="11" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="K20" s="1" t="s">
         <v>64</v>
@@ -5774,26 +3982,26 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E2:E20 F20:J20 F16:J16 G7:G20 J2:J20 I18:I19 I15:I16 F9:J13 I8:I11 F2:J6">
-    <cfRule type="containsText" dxfId="114" priority="5" operator="containsText" text="Safe">
+    <cfRule type="containsText" dxfId="52" priority="5" operator="containsText" text="Safe">
       <formula>NOT(ISERROR(SEARCH("Safe",E2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="113" priority="6" operator="containsText" text="Safe">
+    <cfRule type="containsText" dxfId="51" priority="6" operator="containsText" text="Safe">
       <formula>NOT(ISERROR(SEARCH("Safe",E2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:J20">
-    <cfRule type="containsText" dxfId="112" priority="3" operator="containsText" text="Unsafe">
+    <cfRule type="containsText" dxfId="50" priority="3" operator="containsText" text="Unsafe">
       <formula>NOT(ISERROR(SEARCH("Unsafe",E2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="111" priority="4" operator="containsText" text="Safe">
+    <cfRule type="containsText" dxfId="49" priority="4" operator="containsText" text="Safe">
       <formula>NOT(ISERROR(SEARCH("Safe",E2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:G1048576 I1:J20">
-    <cfRule type="containsText" dxfId="110" priority="1" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="48" priority="1" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="109" priority="2" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="47" priority="2" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",F1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6057,10 +4265,10 @@
       <c r="E9" s="27" t="s">
         <v>119</v>
       </c>
-      <c r="F9" s="35" t="s">
+      <c r="F9" s="31" t="s">
         <v>119</v>
       </c>
-      <c r="G9" s="35" t="s">
+      <c r="G9" s="31" t="s">
         <v>119</v>
       </c>
       <c r="H9" s="28" t="s">
@@ -6151,31 +4359,31 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E2:G12">
-    <cfRule type="containsText" dxfId="108" priority="4" operator="containsText" text="Unsafe">
+    <cfRule type="containsText" dxfId="39" priority="4" operator="containsText" text="Unsafe">
       <formula>NOT(ISERROR(SEARCH("Unsafe",E2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="107" priority="5" operator="containsText" text="Safe">
+    <cfRule type="containsText" dxfId="38" priority="5" operator="containsText" text="Safe">
       <formula>NOT(ISERROR(SEARCH("Safe",E2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:G12">
-    <cfRule type="containsText" dxfId="106" priority="6" operator="containsText" text="Safe">
+    <cfRule type="containsText" dxfId="37" priority="6" operator="containsText" text="Safe">
       <formula>NOT(ISERROR(SEARCH("Safe",E2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="105" priority="7" operator="containsText" text="Safe">
+    <cfRule type="containsText" dxfId="36" priority="7" operator="containsText" text="Safe">
       <formula>NOT(ISERROR(SEARCH("Safe",E2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F1048576 G2">
-    <cfRule type="containsText" dxfId="104" priority="3" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="35" priority="3" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",F1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:G1048576">
-    <cfRule type="containsText" dxfId="103" priority="1" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="34" priority="1" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="102" priority="2" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="33" priority="2" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",F1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6209,17 +4417,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="32" t="s">
         <v>73</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
+      <c r="I1" s="32"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
@@ -6249,7 +4457,7 @@
       <c r="I2" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="K2" s="32" t="s">
+      <c r="K2" s="33" t="s">
         <v>75</v>
       </c>
     </row>
@@ -6281,7 +4489,7 @@
         <f>(Table2[[#This Row],[True Posistive Rate]]+(1 - Table2[[#This Row],[False Positive Rate]])) - 1</f>
         <v>1</v>
       </c>
-      <c r="K3" s="33"/>
+      <c r="K3" s="34"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
@@ -6311,7 +4519,7 @@
         <f>(Table2[[#This Row],[True Posistive Rate]]+(1 - Table2[[#This Row],[False Positive Rate]])) - 1</f>
         <v>1</v>
       </c>
-      <c r="K4" s="33"/>
+      <c r="K4" s="34"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
@@ -6341,7 +4549,7 @@
         <f>(Table2[[#This Row],[True Posistive Rate]]+(1 - Table2[[#This Row],[False Positive Rate]])) - 1</f>
         <v>1</v>
       </c>
-      <c r="K5" s="33"/>
+      <c r="K5" s="34"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
@@ -6371,7 +4579,7 @@
         <f>(Table2[[#This Row],[True Posistive Rate]]+(1 - Table2[[#This Row],[False Positive Rate]])) - 1</f>
         <v>1</v>
       </c>
-      <c r="K6" s="33"/>
+      <c r="K6" s="34"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
@@ -6401,7 +4609,7 @@
         <f>(Table2[[#This Row],[True Posistive Rate]]+(1 - Table2[[#This Row],[False Positive Rate]])) - 1</f>
         <v>1</v>
       </c>
-      <c r="K7" s="33"/>
+      <c r="K7" s="34"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
@@ -6431,7 +4639,7 @@
         <f>(Table2[[#This Row],[True Posistive Rate]]+(1 - Table2[[#This Row],[False Positive Rate]])) - 1</f>
         <v>1</v>
       </c>
-      <c r="K8" s="33"/>
+      <c r="K8" s="34"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
@@ -6461,7 +4669,7 @@
         <f>(Table2[[#This Row],[True Posistive Rate]]+(1 - Table2[[#This Row],[False Positive Rate]])) - 1</f>
         <v>1</v>
       </c>
-      <c r="K9" s="33"/>
+      <c r="K9" s="34"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
@@ -6491,7 +4699,7 @@
         <f>(Table2[[#This Row],[True Posistive Rate]]+(1 - Table2[[#This Row],[False Positive Rate]])) - 1</f>
         <v>0</v>
       </c>
-      <c r="K10" s="33"/>
+      <c r="K10" s="34"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
@@ -6529,7 +4737,7 @@
         <f>ROUND(AVERAGE(I3:I10)*100, 0)</f>
         <v>88</v>
       </c>
-      <c r="K11" s="33"/>
+      <c r="K11" s="34"/>
     </row>
     <row r="12" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="11"/>
@@ -6699,17 +4907,17 @@
       <c r="I27" s="10"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="31" t="s">
+      <c r="A29" s="32" t="s">
         <v>74</v>
       </c>
-      <c r="B29" s="31"/>
-      <c r="C29" s="31"/>
-      <c r="D29" s="31"/>
-      <c r="E29" s="31"/>
-      <c r="F29" s="31"/>
-      <c r="G29" s="31"/>
-      <c r="H29" s="31"/>
-      <c r="I29" s="31"/>
+      <c r="B29" s="32"/>
+      <c r="C29" s="32"/>
+      <c r="D29" s="32"/>
+      <c r="E29" s="32"/>
+      <c r="F29" s="32"/>
+      <c r="G29" s="32"/>
+      <c r="H29" s="32"/>
+      <c r="I29" s="32"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="11" t="s">
@@ -7227,17 +5435,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="35" t="s">
         <v>116</v>
       </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
-      <c r="H1" s="34"/>
-      <c r="I1" s="34"/>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
+      <c r="I1" s="35"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
@@ -7268,7 +5476,7 @@
         <v>72</v>
       </c>
       <c r="J2" s="11"/>
-      <c r="K2" s="32" t="s">
+      <c r="K2" s="33" t="s">
         <v>114</v>
       </c>
     </row>
@@ -7301,7 +5509,7 @@
         <v>0</v>
       </c>
       <c r="J3" s="11"/>
-      <c r="K3" s="33"/>
+      <c r="K3" s="34"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
@@ -7332,7 +5540,7 @@
         <v>0</v>
       </c>
       <c r="J4" s="11"/>
-      <c r="K4" s="33"/>
+      <c r="K4" s="34"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
@@ -7371,7 +5579,7 @@
         <v>0</v>
       </c>
       <c r="J5" s="11"/>
-      <c r="K5" s="33"/>
+      <c r="K5" s="34"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="11"/>
@@ -7384,7 +5592,7 @@
       <c r="H6" s="11"/>
       <c r="I6" s="11"/>
       <c r="J6" s="11"/>
-      <c r="K6" s="33"/>
+      <c r="K6" s="34"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="11"/>
@@ -7397,7 +5605,7 @@
       <c r="H7" s="11"/>
       <c r="I7" s="11"/>
       <c r="J7" s="11"/>
-      <c r="K7" s="33"/>
+      <c r="K7" s="34"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="11"/>
@@ -7410,7 +5618,7 @@
       <c r="H8" s="11"/>
       <c r="I8" s="11"/>
       <c r="J8" s="11"/>
-      <c r="K8" s="33"/>
+      <c r="K8" s="34"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="11"/>
@@ -7423,7 +5631,7 @@
       <c r="H9" s="11"/>
       <c r="I9" s="11"/>
       <c r="J9" s="11"/>
-      <c r="K9" s="33"/>
+      <c r="K9" s="34"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="11"/>
@@ -7436,7 +5644,7 @@
       <c r="H10" s="11"/>
       <c r="I10" s="11"/>
       <c r="J10" s="11"/>
-      <c r="K10" s="33"/>
+      <c r="K10" s="34"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="11"/>
@@ -7449,7 +5657,7 @@
       <c r="H11" s="11"/>
       <c r="I11" s="11"/>
       <c r="J11" s="11"/>
-      <c r="K11" s="33"/>
+      <c r="K11" s="34"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="11"/>
@@ -7654,17 +5862,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="32" t="s">
         <v>73</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
+      <c r="I1" s="32"/>
       <c r="J1" s="11"/>
       <c r="K1" s="11"/>
     </row>
@@ -7697,7 +5905,7 @@
         <v>72</v>
       </c>
       <c r="J2" s="11"/>
-      <c r="K2" s="32" t="s">
+      <c r="K2" s="33" t="s">
         <v>76</v>
       </c>
     </row>
@@ -7730,7 +5938,7 @@
         <v>0</v>
       </c>
       <c r="J3" s="11"/>
-      <c r="K3" s="33"/>
+      <c r="K3" s="34"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
@@ -7761,7 +5969,7 @@
         <v>0</v>
       </c>
       <c r="J4" s="11"/>
-      <c r="K4" s="33"/>
+      <c r="K4" s="34"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
@@ -7792,7 +6000,7 @@
         <v>0</v>
       </c>
       <c r="J5" s="11"/>
-      <c r="K5" s="33"/>
+      <c r="K5" s="34"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
@@ -7821,7 +6029,7 @@
         <v>0</v>
       </c>
       <c r="J6" s="11"/>
-      <c r="K6" s="33"/>
+      <c r="K6" s="34"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
@@ -7852,7 +6060,7 @@
         <v>0</v>
       </c>
       <c r="J7" s="11"/>
-      <c r="K7" s="33"/>
+      <c r="K7" s="34"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
@@ -7883,7 +6091,7 @@
         <v>0</v>
       </c>
       <c r="J8" s="11"/>
-      <c r="K8" s="33"/>
+      <c r="K8" s="34"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
@@ -7914,7 +6122,7 @@
         <v>0</v>
       </c>
       <c r="J9" s="11"/>
-      <c r="K9" s="33"/>
+      <c r="K9" s="34"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
@@ -7945,7 +6153,7 @@
         <v>0</v>
       </c>
       <c r="J10" s="11"/>
-      <c r="K10" s="33"/>
+      <c r="K10" s="34"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
@@ -7984,7 +6192,7 @@
         <v>0</v>
       </c>
       <c r="J11" s="11"/>
-      <c r="K11" s="33"/>
+      <c r="K11" s="34"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="11"/>
@@ -8208,17 +6416,17 @@
       <c r="K28" s="11"/>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="31" t="s">
+      <c r="A29" s="32" t="s">
         <v>74</v>
       </c>
-      <c r="B29" s="31"/>
-      <c r="C29" s="31"/>
-      <c r="D29" s="31"/>
-      <c r="E29" s="31"/>
-      <c r="F29" s="31"/>
-      <c r="G29" s="31"/>
-      <c r="H29" s="31"/>
-      <c r="I29" s="31"/>
+      <c r="B29" s="32"/>
+      <c r="C29" s="32"/>
+      <c r="D29" s="32"/>
+      <c r="E29" s="32"/>
+      <c r="F29" s="32"/>
+      <c r="G29" s="32"/>
+      <c r="H29" s="32"/>
+      <c r="I29" s="32"/>
       <c r="J29" s="11"/>
       <c r="K29" s="11"/>
     </row>
@@ -8781,17 +6989,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="35" t="s">
         <v>115</v>
       </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
-      <c r="H1" s="34"/>
-      <c r="I1" s="34"/>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
+      <c r="I1" s="35"/>
       <c r="J1" s="11"/>
       <c r="K1" s="11"/>
     </row>
@@ -8824,7 +7032,7 @@
         <v>72</v>
       </c>
       <c r="J2" s="11"/>
-      <c r="K2" s="32"/>
+      <c r="K2" s="33"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
@@ -8857,7 +7065,7 @@
         <v>0.25</v>
       </c>
       <c r="J3" s="11"/>
-      <c r="K3" s="33"/>
+      <c r="K3" s="34"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
@@ -8888,7 +7096,7 @@
         <v>0</v>
       </c>
       <c r="J4" s="11"/>
-      <c r="K4" s="33"/>
+      <c r="K4" s="34"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
@@ -8927,7 +7135,7 @@
         <v>13</v>
       </c>
       <c r="J5" s="11"/>
-      <c r="K5" s="33"/>
+      <c r="K5" s="34"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="11"/>
@@ -8940,7 +7148,7 @@
       <c r="H6" s="11"/>
       <c r="I6" s="11"/>
       <c r="J6" s="11"/>
-      <c r="K6" s="33"/>
+      <c r="K6" s="34"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="11"/>
@@ -8953,7 +7161,7 @@
       <c r="H7" s="11"/>
       <c r="I7" s="11"/>
       <c r="J7" s="11"/>
-      <c r="K7" s="33"/>
+      <c r="K7" s="34"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="11"/>
@@ -8966,7 +7174,7 @@
       <c r="H8" s="11"/>
       <c r="I8" s="11"/>
       <c r="J8" s="11"/>
-      <c r="K8" s="33"/>
+      <c r="K8" s="34"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="11"/>
@@ -8979,7 +7187,7 @@
       <c r="H9" s="11"/>
       <c r="I9" s="11"/>
       <c r="J9" s="11"/>
-      <c r="K9" s="33"/>
+      <c r="K9" s="34"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="11"/>
@@ -8992,7 +7200,7 @@
       <c r="H10" s="11"/>
       <c r="I10" s="11"/>
       <c r="J10" s="11"/>
-      <c r="K10" s="33"/>
+      <c r="K10" s="34"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="11"/>
@@ -9005,7 +7213,7 @@
       <c r="H11" s="11"/>
       <c r="I11" s="11"/>
       <c r="J11" s="11"/>
-      <c r="K11" s="33"/>
+      <c r="K11" s="34"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="11"/>

</xml_diff>

<commit_message>
Update graphs for XXE for Contrast 3.4.2
</commit_message>
<xml_diff>
--- a/DotNET Tests and Results.xlsx
+++ b/DotNET Tests and Results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="30" windowWidth="26835" windowHeight="13350"/>
+    <workbookView xWindow="480" yWindow="30" windowWidth="26835" windowHeight="13350" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="XXE Unit Test Cases" sheetId="1" r:id="rId1"/>
@@ -356,9 +356,6 @@
 as well as analyzing the solution in .NET 4.5.1 and 4.5.2 (positives and negatives are different, however)</t>
   </si>
   <si>
-    <t>Contrast did not detect anthing .NET 4.5.1 and 4.5.2 (positives and negatives are different, however)</t>
-  </si>
-  <si>
     <t>Query Type</t>
   </si>
   <si>
@@ -504,6 +501,9 @@
   </si>
   <si>
     <t>Fortify Detection (4.5.2)</t>
+  </si>
+  <si>
+    <t>Updated for Contrast 3.4.2</t>
   </si>
 </sst>
 </file>
@@ -1344,11 +1344,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="92801280"/>
-        <c:axId val="92801856"/>
+        <c:axId val="154405120"/>
+        <c:axId val="154405696"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="92801280"/>
+        <c:axId val="154405120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -1384,13 +1384,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="92801856"/>
+        <c:crossAx val="154405696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.1"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="92801856"/>
+        <c:axId val="154405696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -1421,7 +1421,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="92801280"/>
+        <c:crossAx val="154405120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.1"/>
@@ -1554,11 +1554,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="92803584"/>
-        <c:axId val="92804160"/>
+        <c:axId val="154407424"/>
+        <c:axId val="154408000"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="92803584"/>
+        <c:axId val="154407424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -1594,13 +1594,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="92804160"/>
+        <c:crossAx val="154408000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.1"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="92804160"/>
+        <c:axId val="154408000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -1631,7 +1631,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="92803584"/>
+        <c:crossAx val="154407424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.1"/>
@@ -1764,11 +1764,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="92806464"/>
-        <c:axId val="165167104"/>
+        <c:axId val="154410304"/>
+        <c:axId val="165085184"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="92806464"/>
+        <c:axId val="154410304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -1804,13 +1804,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="165167104"/>
+        <c:crossAx val="165085184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.1"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="165167104"/>
+        <c:axId val="165085184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -1841,7 +1841,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="92806464"/>
+        <c:crossAx val="154410304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.1"/>
@@ -1909,7 +1909,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1974,11 +1974,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="165169984"/>
-        <c:axId val="165170560"/>
+        <c:axId val="165088064"/>
+        <c:axId val="165088640"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="165169984"/>
+        <c:axId val="165088064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -2008,19 +2008,20 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="165170560"/>
+        <c:crossAx val="165088640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.1"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="165170560"/>
+        <c:axId val="165088640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -2045,13 +2046,14 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="165169984"/>
+        <c:crossAx val="165088064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.1"/>
@@ -2119,7 +2121,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>0.625</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2184,11 +2186,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="165172288"/>
-        <c:axId val="165172864"/>
+        <c:axId val="165090368"/>
+        <c:axId val="165090944"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="165172288"/>
+        <c:axId val="165090368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -2218,19 +2220,20 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="165172864"/>
+        <c:crossAx val="165090944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.1"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="165172864"/>
+        <c:axId val="165090944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -2255,13 +2258,14 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="165172288"/>
+        <c:crossAx val="165090368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.1"/>
@@ -2394,11 +2398,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="165683200"/>
-        <c:axId val="165683776"/>
+        <c:axId val="166010880"/>
+        <c:axId val="166011456"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="165683200"/>
+        <c:axId val="166010880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -2434,13 +2438,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="165683776"/>
+        <c:crossAx val="166011456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.1"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="165683776"/>
+        <c:axId val="166011456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -2471,7 +2475,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="165683200"/>
+        <c:crossAx val="166010880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.1"/>
@@ -3138,9 +3142,9 @@
   </sheetPr>
   <dimension ref="A1:K39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H28" sqref="H28"/>
+      <selection pane="bottomLeft" activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3159,7 +3163,7 @@
   <sheetData>
     <row r="1" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>0</v>
@@ -3174,19 +3178,19 @@
         <v>5</v>
       </c>
       <c r="F1" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="G1" s="5" t="s">
         <v>122</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>123</v>
       </c>
       <c r="H1" s="5" t="s">
         <v>6</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="J1" s="5" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>1</v>
@@ -3209,19 +3213,19 @@
         <v>3</v>
       </c>
       <c r="F2" s="11" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G2" s="11" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>3</v>
       </c>
       <c r="I2" s="11" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="J2" s="11" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="K2" s="1" t="s">
         <v>46</v>
@@ -3244,19 +3248,19 @@
         <v>3</v>
       </c>
       <c r="F3" s="11" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G3" s="11" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>3</v>
       </c>
       <c r="I3" s="11" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="J3" s="11" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="K3" s="1" t="s">
         <v>47</v>
@@ -3279,19 +3283,19 @@
         <v>2</v>
       </c>
       <c r="F4" s="11" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G4" s="11" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>2</v>
       </c>
       <c r="I4" s="11" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="J4" s="11" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="K4" s="1" t="s">
         <v>48</v>
@@ -3314,19 +3318,19 @@
         <v>3</v>
       </c>
       <c r="F5" s="11" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G5" s="11" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H5" s="2" t="s">
         <v>3</v>
       </c>
       <c r="I5" s="11" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="J5" s="11" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="K5" s="1" t="s">
         <v>49</v>
@@ -3349,19 +3353,19 @@
         <v>2</v>
       </c>
       <c r="F6" s="11" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G6" s="11" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H6" s="2" t="s">
         <v>2</v>
       </c>
       <c r="I6" s="11" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="J6" s="11" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="K6" s="1" t="s">
         <v>50</v>
@@ -3384,19 +3388,19 @@
         <v>2</v>
       </c>
       <c r="F7" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="G7" s="11" t="s">
         <v>120</v>
-      </c>
-      <c r="G7" s="11" t="s">
-        <v>121</v>
       </c>
       <c r="H7" s="5" t="s">
         <v>3</v>
       </c>
       <c r="I7" s="5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="J7" s="11" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="K7" s="1" t="s">
         <v>51</v>
@@ -3419,19 +3423,19 @@
         <v>3</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G8" s="11" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H8" s="5" t="s">
         <v>3</v>
       </c>
       <c r="I8" s="11" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="J8" s="11" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="K8" s="1" t="s">
         <v>52</v>
@@ -3454,19 +3458,19 @@
         <v>2</v>
       </c>
       <c r="F9" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="G9" s="11" t="s">
         <v>120</v>
-      </c>
-      <c r="G9" s="11" t="s">
-        <v>121</v>
       </c>
       <c r="H9" s="2" t="s">
         <v>2</v>
       </c>
       <c r="I9" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="J9" s="11" t="s">
         <v>120</v>
-      </c>
-      <c r="J9" s="11" t="s">
-        <v>121</v>
       </c>
       <c r="K9" s="1" t="s">
         <v>53</v>
@@ -3489,19 +3493,19 @@
         <v>3</v>
       </c>
       <c r="F10" s="11" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G10" s="11" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H10" s="2" t="s">
         <v>3</v>
       </c>
       <c r="I10" s="11" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="J10" s="11" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="K10" s="1" t="s">
         <v>54</v>
@@ -3524,19 +3528,19 @@
         <v>2</v>
       </c>
       <c r="F11" s="11" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G11" s="11" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H11" s="2" t="s">
         <v>2</v>
       </c>
       <c r="I11" s="11" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="J11" s="11" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="K11" s="1" t="s">
         <v>56</v>
@@ -3559,19 +3563,19 @@
         <v>3</v>
       </c>
       <c r="F12" s="11" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G12" s="11" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H12" s="2" t="s">
         <v>3</v>
       </c>
       <c r="I12" s="11" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="J12" s="11" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="K12" s="1" t="s">
         <v>55</v>
@@ -3594,19 +3598,19 @@
         <v>3</v>
       </c>
       <c r="F13" s="11" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G13" s="11" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H13" s="2" t="s">
         <v>3</v>
       </c>
       <c r="I13" s="11" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="J13" s="11" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="K13" s="1" t="s">
         <v>57</v>
@@ -3629,19 +3633,19 @@
         <v>2</v>
       </c>
       <c r="F14" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="G14" s="11" t="s">
         <v>120</v>
-      </c>
-      <c r="G14" s="11" t="s">
-        <v>121</v>
       </c>
       <c r="H14" s="5" t="s">
         <v>3</v>
       </c>
       <c r="I14" s="5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="J14" s="11" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="K14" s="1" t="s">
         <v>58</v>
@@ -3664,19 +3668,19 @@
         <v>3</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G15" s="11" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H15" s="5" t="s">
         <v>3</v>
       </c>
       <c r="I15" s="11" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="J15" s="11" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="K15" s="1" t="s">
         <v>59</v>
@@ -3699,19 +3703,19 @@
         <v>2</v>
       </c>
       <c r="F16" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="G16" s="11" t="s">
         <v>120</v>
-      </c>
-      <c r="G16" s="11" t="s">
-        <v>121</v>
       </c>
       <c r="H16" s="2" t="s">
         <v>2</v>
       </c>
       <c r="I16" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="J16" s="11" t="s">
         <v>120</v>
-      </c>
-      <c r="J16" s="11" t="s">
-        <v>121</v>
       </c>
       <c r="K16" s="1" t="s">
         <v>60</v>
@@ -3734,19 +3738,19 @@
         <v>2</v>
       </c>
       <c r="F17" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="G17" s="11" t="s">
         <v>120</v>
-      </c>
-      <c r="G17" s="11" t="s">
-        <v>121</v>
       </c>
       <c r="H17" s="5" t="s">
         <v>3</v>
       </c>
       <c r="I17" s="5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="J17" s="11" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="K17" s="1" t="s">
         <v>61</v>
@@ -3769,19 +3773,19 @@
         <v>3</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G18" s="11" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H18" s="5" t="s">
         <v>3</v>
       </c>
       <c r="I18" s="11" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="J18" s="11" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="K18" s="1" t="s">
         <v>62</v>
@@ -3804,19 +3808,19 @@
         <v>3</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G19" s="11" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H19" s="5" t="s">
         <v>3</v>
       </c>
       <c r="I19" s="11" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="J19" s="11" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="K19" s="1" t="s">
         <v>63</v>
@@ -3839,19 +3843,19 @@
         <v>2</v>
       </c>
       <c r="F20" s="11" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G20" s="11" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H20" s="2" t="s">
         <v>2</v>
       </c>
       <c r="I20" s="11" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="J20" s="11" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="K20" s="1" t="s">
         <v>64</v>
@@ -4035,10 +4039,10 @@
   <sheetData>
     <row r="1" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="22" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B1" s="22" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C1" s="22" t="s">
         <v>34</v>
@@ -4047,13 +4051,13 @@
         <v>4</v>
       </c>
       <c r="E1" s="22" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F1" s="22" t="s">
+        <v>116</v>
+      </c>
+      <c r="G1" s="22" t="s">
         <v>117</v>
-      </c>
-      <c r="G1" s="22" t="s">
-        <v>118</v>
       </c>
       <c r="H1" s="23" t="s">
         <v>1</v>
@@ -4065,25 +4069,25 @@
         <v>1</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E2" s="16" t="s">
         <v>3</v>
       </c>
       <c r="F2" s="17" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G2" s="17" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H2" s="20" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="I2" s="11"/>
     </row>
@@ -4092,25 +4096,25 @@
         <v>2</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C3" s="17" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D3" s="17" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E3" s="16" t="s">
         <v>2</v>
       </c>
       <c r="F3" s="24" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G3" s="24" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H3" s="21" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="I3" s="11"/>
     </row>
@@ -4119,25 +4123,25 @@
         <v>3</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C4" s="16" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D4" s="16" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E4" s="16" t="s">
         <v>2</v>
       </c>
       <c r="F4" s="24" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G4" s="17" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H4" s="20" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I4" s="11"/>
     </row>
@@ -4146,25 +4150,25 @@
         <v>4</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D5" s="17" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E5" s="16" t="s">
         <v>2</v>
       </c>
       <c r="F5" s="24" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G5" s="17" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H5" s="21" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="I5" s="11"/>
     </row>
@@ -4173,25 +4177,25 @@
         <v>5</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C6" s="16" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D6" s="17" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E6" s="16" t="s">
         <v>2</v>
       </c>
       <c r="F6" s="24" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G6" s="17" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H6" s="20" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I6" s="11"/>
     </row>
@@ -4200,25 +4204,25 @@
         <v>6</v>
       </c>
       <c r="B7" s="17" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C7" s="18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D7" s="17" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E7" s="19" t="s">
         <v>3</v>
       </c>
       <c r="F7" s="17" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G7" s="17" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H7" s="21" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="I7" s="11"/>
     </row>
@@ -4227,25 +4231,25 @@
         <v>7</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C8" s="16" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D8" s="16" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E8" s="19" t="s">
         <v>3</v>
       </c>
       <c r="F8" s="17" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G8" s="17" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H8" s="21" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="I8" s="11"/>
     </row>
@@ -4254,25 +4258,25 @@
         <v>8</v>
       </c>
       <c r="B9" s="26" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C9" s="26" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D9" s="26" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E9" s="27" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F9" s="31" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G9" s="31" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H9" s="28" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I9" s="11"/>
     </row>
@@ -4281,25 +4285,25 @@
         <v>9</v>
       </c>
       <c r="B10" s="17" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C10" s="16" t="s">
+        <v>101</v>
+      </c>
+      <c r="D10" s="16" t="s">
         <v>102</v>
-      </c>
-      <c r="D10" s="16" t="s">
-        <v>103</v>
       </c>
       <c r="E10" s="17" t="s">
         <v>2</v>
       </c>
       <c r="F10" s="17" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G10" s="17" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H10" s="20" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="I10" s="11"/>
     </row>
@@ -4308,25 +4312,25 @@
         <v>10</v>
       </c>
       <c r="B11" s="17" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C11" s="17" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D11" s="17" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E11" s="17" t="s">
         <v>2</v>
       </c>
       <c r="F11" s="17" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G11" s="17" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H11" s="30" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I11" s="11"/>
     </row>
@@ -4335,25 +4339,25 @@
         <v>11</v>
       </c>
       <c r="B12" s="17" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C12" s="24" t="s">
+        <v>110</v>
+      </c>
+      <c r="D12" s="24" t="s">
         <v>111</v>
-      </c>
-      <c r="D12" s="24" t="s">
-        <v>112</v>
       </c>
       <c r="E12" s="24" t="s">
         <v>3</v>
       </c>
       <c r="F12" s="24" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G12" s="24" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H12" s="25" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="I12" s="11"/>
     </row>
@@ -5436,7 +5440,7 @@
   <sheetData>
     <row r="1" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="35" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B1" s="35"/>
       <c r="C1" s="35"/>
@@ -5449,7 +5453,7 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B2" s="11" t="s">
         <v>65</v>
@@ -5477,12 +5481,12 @@
       </c>
       <c r="J2" s="11"/>
       <c r="K2" s="33" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B3" s="11"/>
       <c r="C3" s="11">
@@ -5513,7 +5517,7 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B4" s="11"/>
       <c r="C4" s="11">
@@ -5843,8 +5847,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K55"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5906,17 +5910,17 @@
       </c>
       <c r="J2" s="11"/>
       <c r="K2" s="33" t="s">
-        <v>76</v>
+        <v>125</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="11"/>
-      <c r="C3" s="11">
-        <v>1</v>
-      </c>
+      <c r="B3" s="11">
+        <v>1</v>
+      </c>
+      <c r="C3" s="11"/>
       <c r="D3" s="11">
         <v>2</v>
       </c>
@@ -5927,7 +5931,7 @@
       </c>
       <c r="G3" s="13">
         <f>IF(Table28[[#This Row],[True Positive]]+Table28[[#This Row],[False Negative]]=0,0,Table28[[#This Row],[True Positive]]/(Table28[[#This Row],[True Positive]]+Table28[[#This Row],[False Negative]]))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H3" s="13">
         <f>Table28[[#This Row],[False Positive]]/(Table28[[#This Row],[False Positive]]+Table28[[#This Row],[True Negative]])</f>
@@ -5935,7 +5939,7 @@
       </c>
       <c r="I3" s="13">
         <f>(Table28[[#This Row],[True Posistive Rate]]+(1 - Table28[[#This Row],[False Positive Rate]])) - 1</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J3" s="11"/>
       <c r="K3" s="34"/>
@@ -5944,10 +5948,10 @@
       <c r="A4" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="11"/>
-      <c r="C4" s="11">
-        <v>1</v>
-      </c>
+      <c r="B4" s="11">
+        <v>1</v>
+      </c>
+      <c r="C4" s="11"/>
       <c r="D4" s="11">
         <v>1</v>
       </c>
@@ -5958,7 +5962,7 @@
       </c>
       <c r="G4" s="13">
         <f>IF(Table28[[#This Row],[True Positive]]+Table28[[#This Row],[False Negative]]=0,0,Table28[[#This Row],[True Positive]]/(Table28[[#This Row],[True Positive]]+Table28[[#This Row],[False Negative]]))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H4" s="13">
         <f>Table28[[#This Row],[False Positive]]/(Table28[[#This Row],[False Positive]]+Table28[[#This Row],[True Negative]])</f>
@@ -5966,7 +5970,7 @@
       </c>
       <c r="I4" s="13">
         <f>(Table28[[#This Row],[True Posistive Rate]]+(1 - Table28[[#This Row],[False Positive Rate]])) - 1</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J4" s="11"/>
       <c r="K4" s="34"/>
@@ -6035,10 +6039,10 @@
       <c r="A7" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="11"/>
-      <c r="C7" s="11">
-        <v>1</v>
-      </c>
+      <c r="B7" s="11">
+        <v>1</v>
+      </c>
+      <c r="C7" s="11"/>
       <c r="D7" s="11">
         <v>1</v>
       </c>
@@ -6049,7 +6053,7 @@
       </c>
       <c r="G7" s="13">
         <f>IF(Table28[[#This Row],[True Positive]]+Table28[[#This Row],[False Negative]]=0,0,Table28[[#This Row],[True Positive]]/(Table28[[#This Row],[True Positive]]+Table28[[#This Row],[False Negative]]))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H7" s="13">
         <f>Table28[[#This Row],[False Positive]]/(Table28[[#This Row],[False Positive]]+Table28[[#This Row],[True Negative]])</f>
@@ -6057,7 +6061,7 @@
       </c>
       <c r="I7" s="13">
         <f>(Table28[[#This Row],[True Posistive Rate]]+(1 - Table28[[#This Row],[False Positive Rate]])) - 1</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J7" s="11"/>
       <c r="K7" s="34"/>
@@ -6128,10 +6132,10 @@
       <c r="A10" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="11"/>
-      <c r="C10" s="11">
-        <v>1</v>
-      </c>
+      <c r="B10" s="11">
+        <v>1</v>
+      </c>
+      <c r="C10" s="11"/>
       <c r="D10" s="11">
         <v>1</v>
       </c>
@@ -6142,7 +6146,7 @@
       </c>
       <c r="G10" s="13">
         <f>IF(Table28[[#This Row],[True Positive]]+Table28[[#This Row],[False Negative]]=0,0,Table28[[#This Row],[True Positive]]/(Table28[[#This Row],[True Positive]]+Table28[[#This Row],[False Negative]]))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H10" s="13">
         <f>Table28[[#This Row],[False Positive]]/(Table28[[#This Row],[False Positive]]+Table28[[#This Row],[True Negative]])</f>
@@ -6150,7 +6154,7 @@
       </c>
       <c r="I10" s="13">
         <f>(Table28[[#This Row],[True Posistive Rate]]+(1 - Table28[[#This Row],[False Positive Rate]])) - 1</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J10" s="11"/>
       <c r="K10" s="34"/>
@@ -6161,11 +6165,11 @@
       </c>
       <c r="B11" s="9">
         <f>SUM(B3:B10)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C11" s="9">
         <f t="shared" ref="C11:F11" si="0">SUM(C3:C10)</f>
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D11" s="9">
         <f t="shared" si="0"/>
@@ -6181,7 +6185,7 @@
       </c>
       <c r="G11" s="9">
         <f>AVERAGE(G3:G10)</f>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="H11" s="9">
         <f>AVERAGE(H3:H10)</f>
@@ -6189,7 +6193,7 @@
       </c>
       <c r="I11" s="9">
         <f>ROUND(AVERAGE(I3:I10)*100, 0)</f>
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="J11" s="11"/>
       <c r="K11" s="34"/>
@@ -6465,10 +6469,10 @@
       <c r="A31" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="B31" s="11"/>
-      <c r="C31" s="11">
-        <v>1</v>
-      </c>
+      <c r="B31" s="11">
+        <v>1</v>
+      </c>
+      <c r="C31" s="11"/>
       <c r="D31" s="11">
         <v>2</v>
       </c>
@@ -6479,7 +6483,7 @@
       </c>
       <c r="G31" s="13">
         <f>IF(Table279[[#This Row],[True Positive]]+Table279[[#This Row],[False Negative]]=0,0,Table279[[#This Row],[True Positive]]/(Table279[[#This Row],[True Positive]]+Table279[[#This Row],[False Negative]]))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H31" s="13">
         <f>Table279[[#This Row],[False Positive]]/(Table279[[#This Row],[False Positive]]+Table279[[#This Row],[True Negative]])</f>
@@ -6487,7 +6491,7 @@
       </c>
       <c r="I31" s="13">
         <f>(Table279[[#This Row],[True Posistive Rate]]+(1 - Table279[[#This Row],[False Positive Rate]])) - 1</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J31" s="11"/>
       <c r="K31" s="11"/>
@@ -6496,10 +6500,10 @@
       <c r="A32" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="B32" s="11"/>
-      <c r="C32" s="11">
-        <v>1</v>
-      </c>
+      <c r="B32" s="11">
+        <v>1</v>
+      </c>
+      <c r="C32" s="11"/>
       <c r="D32" s="11">
         <v>1</v>
       </c>
@@ -6510,7 +6514,7 @@
       </c>
       <c r="G32" s="13">
         <f>IF(Table279[[#This Row],[True Positive]]+Table279[[#This Row],[False Negative]]=0,0,Table279[[#This Row],[True Positive]]/(Table279[[#This Row],[True Positive]]+Table279[[#This Row],[False Negative]]))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H32" s="13">
         <f>Table279[[#This Row],[False Positive]]/(Table279[[#This Row],[False Positive]]+Table279[[#This Row],[True Negative]])</f>
@@ -6518,7 +6522,7 @@
       </c>
       <c r="I32" s="13">
         <f>(Table279[[#This Row],[True Posistive Rate]]+(1 - Table279[[#This Row],[False Positive Rate]])) - 1</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J32" s="11"/>
       <c r="K32" s="11"/>
@@ -6527,10 +6531,10 @@
       <c r="A33" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="B33" s="11"/>
-      <c r="C33" s="11">
-        <v>1</v>
-      </c>
+      <c r="B33" s="11">
+        <v>1</v>
+      </c>
+      <c r="C33" s="11"/>
       <c r="D33" s="11">
         <v>2</v>
       </c>
@@ -6541,7 +6545,7 @@
       </c>
       <c r="G33" s="13">
         <f>IF(Table279[[#This Row],[True Positive]]+Table279[[#This Row],[False Negative]]=0,0,Table279[[#This Row],[True Positive]]/(Table279[[#This Row],[True Positive]]+Table279[[#This Row],[False Negative]]))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H33" s="13">
         <f>Table279[[#This Row],[False Positive]]/(Table279[[#This Row],[False Positive]]+Table279[[#This Row],[True Negative]])</f>
@@ -6549,7 +6553,7 @@
       </c>
       <c r="I33" s="13">
         <f>(Table279[[#This Row],[True Posistive Rate]]+(1 - Table279[[#This Row],[False Positive Rate]])) - 1</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J33" s="11"/>
       <c r="K33" s="11"/>
@@ -6587,10 +6591,10 @@
       <c r="A35" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B35" s="11"/>
-      <c r="C35" s="11">
-        <v>1</v>
-      </c>
+      <c r="B35" s="11">
+        <v>1</v>
+      </c>
+      <c r="C35" s="11"/>
       <c r="D35" s="11">
         <v>1</v>
       </c>
@@ -6601,7 +6605,7 @@
       </c>
       <c r="G35" s="13">
         <f>IF(Table279[[#This Row],[True Positive]]+Table279[[#This Row],[False Negative]]=0,0,Table279[[#This Row],[True Positive]]/(Table279[[#This Row],[True Positive]]+Table279[[#This Row],[False Negative]]))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H35" s="13">
         <f>Table279[[#This Row],[False Positive]]/(Table279[[#This Row],[False Positive]]+Table279[[#This Row],[True Negative]])</f>
@@ -6609,7 +6613,7 @@
       </c>
       <c r="I35" s="13">
         <f>(Table279[[#This Row],[True Posistive Rate]]+(1 - Table279[[#This Row],[False Positive Rate]])) - 1</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J35" s="11"/>
       <c r="K35" s="11"/>
@@ -6678,10 +6682,10 @@
       <c r="A38" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B38" s="11"/>
-      <c r="C38" s="11">
-        <v>1</v>
-      </c>
+      <c r="B38" s="11">
+        <v>1</v>
+      </c>
+      <c r="C38" s="11"/>
       <c r="D38" s="11">
         <v>1</v>
       </c>
@@ -6692,7 +6696,7 @@
       </c>
       <c r="G38" s="13">
         <f>IF(Table279[[#This Row],[True Positive]]+Table279[[#This Row],[False Negative]]=0,0,Table279[[#This Row],[True Positive]]/(Table279[[#This Row],[True Positive]]+Table279[[#This Row],[False Negative]]))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H38" s="13">
         <f>Table279[[#This Row],[False Positive]]/(Table279[[#This Row],[False Positive]]+Table279[[#This Row],[True Negative]])</f>
@@ -6700,7 +6704,7 @@
       </c>
       <c r="I38" s="13">
         <f>(Table279[[#This Row],[True Posistive Rate]]+(1 - Table279[[#This Row],[False Positive Rate]])) - 1</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J38" s="11"/>
       <c r="K38" s="11"/>
@@ -6711,11 +6715,11 @@
       </c>
       <c r="B39" s="9">
         <f>SUM(B31:B38)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C39" s="9">
         <f t="shared" ref="C39:F39" si="1">SUM(C31:C38)</f>
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D39" s="9">
         <f t="shared" si="1"/>
@@ -6731,7 +6735,7 @@
       </c>
       <c r="G39" s="9">
         <f>AVERAGE(G31:G38)</f>
-        <v>0</v>
+        <v>0.625</v>
       </c>
       <c r="H39" s="9">
         <f>AVERAGE(H31:H38)</f>
@@ -6739,7 +6743,7 @@
       </c>
       <c r="I39" s="9">
         <f>ROUND(AVERAGE(I31:I38)*100, 0)</f>
-        <v>0</v>
+        <v>63</v>
       </c>
       <c r="J39" s="11"/>
       <c r="K39" s="11"/>
@@ -6990,7 +6994,7 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="35" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B1" s="35"/>
       <c r="C1" s="35"/>
@@ -7005,7 +7009,7 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B2" s="11" t="s">
         <v>65</v>
@@ -7036,7 +7040,7 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B3" s="11">
         <v>1</v>
@@ -7069,7 +7073,7 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B4" s="11"/>
       <c r="C4" s="11">

</xml_diff>

<commit_message>
Update with Contrast 3.4.4 results
</commit_message>
<xml_diff>
--- a/DotNET Tests and Results.xlsx
+++ b/DotNET Tests and Results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="30" windowWidth="26835" windowHeight="13350"/>
+    <workbookView xWindow="480" yWindow="30" windowWidth="26835" windowHeight="13350" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -797,6 +797,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -809,13 +810,218 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Total" xfId="1" builtinId="25"/>
   </cellStyles>
-  <dxfs count="73">
+  <dxfs count="92">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="double">
+          <color rgb="FF4F81BD"/>
+        </bottom>
+      </border>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -860,9 +1066,117 @@
     <dxf>
       <border outline="0">
         <bottom style="double">
-          <color rgb="FF4F81BD"/>
+          <color theme="4"/>
         </bottom>
       </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="double">
+          <color theme="4"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="double">
+          <color theme="4"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="double">
+          <color theme="4"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="double">
+          <color theme="4"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="double">
+          <color theme="4"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="double">
+          <color theme="4"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1154,130 +1468,6 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="double">
-          <color theme="4"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="double">
-          <color theme="4"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="double">
-          <color theme="4"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="double">
-          <color theme="4"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="double">
-          <color theme="4"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="double">
-          <color theme="4"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="double">
-          <color theme="4"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1403,11 +1593,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="161286400"/>
-        <c:axId val="161286976"/>
+        <c:axId val="86985536"/>
+        <c:axId val="86986112"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="161286400"/>
+        <c:axId val="86985536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -1444,13 +1634,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="161286976"/>
+        <c:crossAx val="86986112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.1"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="161286976"/>
+        <c:axId val="86986112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -1482,7 +1672,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="161286400"/>
+        <c:crossAx val="86985536"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.1"/>
@@ -1615,11 +1805,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="173113920"/>
-        <c:axId val="173120832"/>
+        <c:axId val="98275264"/>
+        <c:axId val="98275840"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="173113920"/>
+        <c:axId val="98275264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -1656,13 +1846,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="173120832"/>
+        <c:crossAx val="98275840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.1"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="173120832"/>
+        <c:axId val="98275840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -1694,7 +1884,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="173113920"/>
+        <c:crossAx val="98275264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.1"/>
@@ -1827,11 +2017,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="161288704"/>
-        <c:axId val="161289280"/>
+        <c:axId val="86987840"/>
+        <c:axId val="86988416"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="161288704"/>
+        <c:axId val="86987840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -1868,13 +2058,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="161289280"/>
+        <c:crossAx val="86988416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.1"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="161289280"/>
+        <c:axId val="86988416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -1906,7 +2096,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="161288704"/>
+        <c:crossAx val="86987840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.1"/>
@@ -2039,11 +2229,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="161291584"/>
-        <c:axId val="171982848"/>
+        <c:axId val="97337344"/>
+        <c:axId val="97337920"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="161291584"/>
+        <c:axId val="97337344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -2080,13 +2270,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="171982848"/>
+        <c:crossAx val="97337920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.1"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="171982848"/>
+        <c:axId val="97337920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -2118,7 +2308,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="161291584"/>
+        <c:crossAx val="97337344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.1"/>
@@ -2251,11 +2441,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="139581632"/>
-        <c:axId val="139582208"/>
+        <c:axId val="97340224"/>
+        <c:axId val="97340800"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="139581632"/>
+        <c:axId val="97340224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -2285,20 +2475,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="139582208"/>
+        <c:crossAx val="97340800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.1"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="139582208"/>
+        <c:axId val="97340800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -2323,14 +2512,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="139581632"/>
+        <c:crossAx val="97340224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.1"/>
@@ -2463,11 +2651,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="67296576"/>
-        <c:axId val="103275264"/>
+        <c:axId val="97343104"/>
+        <c:axId val="97343680"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="67296576"/>
+        <c:axId val="97343104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -2497,20 +2685,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="103275264"/>
+        <c:crossAx val="97343680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.1"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="103275264"/>
+        <c:axId val="97343680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -2535,14 +2722,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="67296576"/>
+        <c:crossAx val="97343104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.1"/>
@@ -2675,11 +2861,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="171985728"/>
-        <c:axId val="171986304"/>
+        <c:axId val="97723520"/>
+        <c:axId val="97724096"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="171985728"/>
+        <c:axId val="97723520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -2716,13 +2902,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="171986304"/>
+        <c:crossAx val="97724096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.1"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="171986304"/>
+        <c:axId val="97724096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -2754,7 +2940,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="171985728"/>
+        <c:crossAx val="97723520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.1"/>
@@ -2822,7 +3008,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>0.625</c:v>
+                  <c:v>0.75</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2887,11 +3073,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="171988032"/>
-        <c:axId val="171988608"/>
+        <c:axId val="97725824"/>
+        <c:axId val="97726400"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="171988032"/>
+        <c:axId val="97725824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -2928,13 +3114,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="171988608"/>
+        <c:crossAx val="97726400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.1"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="171988608"/>
+        <c:axId val="97726400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -2966,7 +3152,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="171988032"/>
+        <c:crossAx val="97725824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.1"/>
@@ -3034,7 +3220,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>0.125</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3099,11 +3285,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="172498944"/>
-        <c:axId val="172499520"/>
+        <c:axId val="97728704"/>
+        <c:axId val="97729280"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="172498944"/>
+        <c:axId val="97728704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -3140,13 +3326,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="172499520"/>
+        <c:crossAx val="97729280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.1"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="172499520"/>
+        <c:axId val="97729280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -3178,7 +3364,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="172498944"/>
+        <c:crossAx val="97728704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.1"/>
@@ -3234,7 +3420,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3311,11 +3497,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="67277888"/>
-        <c:axId val="67278464"/>
+        <c:axId val="98272384"/>
+        <c:axId val="98272960"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="67277888"/>
+        <c:axId val="98272384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -3352,13 +3538,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="67278464"/>
+        <c:crossAx val="98272960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.1"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="67278464"/>
+        <c:axId val="98272960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -3390,7 +3576,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="67277888"/>
+        <c:crossAx val="98272384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.1"/>
@@ -3769,7 +3955,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:I39" totalsRowShown="0" headerRowDxfId="72">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:I39" totalsRowShown="0" headerRowDxfId="62">
   <autoFilter ref="A1:I39"/>
   <tableColumns count="9">
     <tableColumn id="1" name="Test"/>
@@ -3778,16 +3964,16 @@
     <tableColumn id="12" name="Test Type"/>
     <tableColumn id="3" name="File Name"/>
     <tableColumn id="4" name="Safety"/>
-    <tableColumn id="8" name="Fortify Detection" dataDxfId="71"/>
-    <tableColumn id="9" name="Contrast Detection" dataDxfId="70"/>
-    <tableColumn id="6" name="Test Description" dataDxfId="69"/>
+    <tableColumn id="8" name="Fortify Detection" dataDxfId="61"/>
+    <tableColumn id="9" name="Contrast Detection" dataDxfId="60"/>
+    <tableColumn id="6" name="Test Description" dataDxfId="59"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Table26411" displayName="Table26411" ref="A2:I4" totalsRowShown="0" tableBorderDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Table26411" displayName="Table26411" ref="A2:I4" totalsRowShown="0" tableBorderDxfId="26">
   <autoFilter ref="A2:I4"/>
   <tableColumns count="9">
     <tableColumn id="1" name="XPath Library"/>
@@ -3796,16 +3982,16 @@
     <tableColumn id="4" name="True Negative"/>
     <tableColumn id="5" name="False Positive"/>
     <tableColumn id="6" name="Total"/>
-    <tableColumn id="7" name="True Posistive Rate" dataDxfId="10"/>
-    <tableColumn id="8" name="False Positive Rate" dataDxfId="9"/>
-    <tableColumn id="9" name="Score" dataDxfId="8"/>
+    <tableColumn id="7" name="True Posistive Rate" dataDxfId="25"/>
+    <tableColumn id="8" name="False Positive Rate" dataDxfId="24"/>
+    <tableColumn id="9" name="Score" dataDxfId="23"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="Table2641213" displayName="Table2641213" ref="A2:I4" totalsRowShown="0" tableBorderDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="Table2641213" displayName="Table2641213" ref="A2:I4" totalsRowShown="0" tableBorderDxfId="22">
   <autoFilter ref="A2:I4"/>
   <tableColumns count="9">
     <tableColumn id="1" name="XQuery Library"/>
@@ -3814,16 +4000,16 @@
     <tableColumn id="4" name="True Negative"/>
     <tableColumn id="5" name="False Positive"/>
     <tableColumn id="6" name="Total"/>
-    <tableColumn id="7" name="True Posistive Rate" dataDxfId="2"/>
-    <tableColumn id="8" name="False Positive Rate" dataDxfId="1"/>
-    <tableColumn id="9" name="Score" dataDxfId="0"/>
+    <tableColumn id="7" name="True Posistive Rate" dataDxfId="21"/>
+    <tableColumn id="8" name="False Positive Rate" dataDxfId="20"/>
+    <tableColumn id="9" name="Score" dataDxfId="19"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A2:I11" totalsRowShown="0" tableBorderDxfId="68">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A2:I11" totalsRowShown="0" tableBorderDxfId="58">
   <autoFilter ref="A2:I11"/>
   <tableColumns count="9">
     <tableColumn id="1" name="XML Parser"/>
@@ -3832,16 +4018,16 @@
     <tableColumn id="4" name="True Negative"/>
     <tableColumn id="5" name="False Positive"/>
     <tableColumn id="6" name="Total"/>
-    <tableColumn id="7" name="True Posistive Rate" dataDxfId="67"/>
-    <tableColumn id="8" name="False Positive Rate" dataDxfId="66"/>
-    <tableColumn id="9" name="Score" dataDxfId="65"/>
+    <tableColumn id="7" name="True Posistive Rate" dataDxfId="57"/>
+    <tableColumn id="8" name="False Positive Rate" dataDxfId="56"/>
+    <tableColumn id="9" name="Score" dataDxfId="55"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table27" displayName="Table27" ref="A30:I39" totalsRowShown="0" tableBorderDxfId="64">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table27" displayName="Table27" ref="A30:I39" totalsRowShown="0" tableBorderDxfId="54">
   <autoFilter ref="A30:I39"/>
   <tableColumns count="9">
     <tableColumn id="1" name="XML Parser"/>
@@ -3850,16 +4036,16 @@
     <tableColumn id="4" name="True Negative"/>
     <tableColumn id="5" name="False Positive"/>
     <tableColumn id="6" name="Total"/>
-    <tableColumn id="7" name="True Posistive Rate" dataDxfId="63"/>
-    <tableColumn id="8" name="False Positive Rate" dataDxfId="62"/>
-    <tableColumn id="9" name="Score" dataDxfId="61"/>
+    <tableColumn id="7" name="True Posistive Rate" dataDxfId="53"/>
+    <tableColumn id="8" name="False Positive Rate" dataDxfId="52"/>
+    <tableColumn id="9" name="Score" dataDxfId="51"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table26" displayName="Table26" ref="A2:I5" totalsRowShown="0" tableBorderDxfId="60">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table26" displayName="Table26" ref="A2:I5" totalsRowShown="0" tableBorderDxfId="50">
   <autoFilter ref="A2:I5"/>
   <tableColumns count="9">
     <tableColumn id="1" name="Query Type"/>
@@ -3868,16 +4054,16 @@
     <tableColumn id="4" name="True Negative"/>
     <tableColumn id="5" name="False Positive"/>
     <tableColumn id="6" name="Total"/>
-    <tableColumn id="7" name="True Posistive Rate" dataDxfId="59"/>
-    <tableColumn id="8" name="False Positive Rate" dataDxfId="58"/>
-    <tableColumn id="9" name="Score" dataDxfId="57"/>
+    <tableColumn id="7" name="True Posistive Rate" dataDxfId="49"/>
+    <tableColumn id="8" name="False Positive Rate" dataDxfId="48"/>
+    <tableColumn id="9" name="Score" dataDxfId="47"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table264" displayName="Table264" ref="A2:I4" totalsRowShown="0" tableBorderDxfId="44">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table264" displayName="Table264" ref="A2:I4" totalsRowShown="0" tableBorderDxfId="46">
   <autoFilter ref="A2:I4"/>
   <tableColumns count="9">
     <tableColumn id="1" name="XPath Library"/>
@@ -3886,16 +4072,16 @@
     <tableColumn id="4" name="True Negative"/>
     <tableColumn id="5" name="False Positive"/>
     <tableColumn id="6" name="Total"/>
-    <tableColumn id="7" name="True Posistive Rate" dataDxfId="43"/>
-    <tableColumn id="8" name="False Positive Rate" dataDxfId="42"/>
-    <tableColumn id="9" name="Score" dataDxfId="41"/>
+    <tableColumn id="7" name="True Posistive Rate" dataDxfId="45"/>
+    <tableColumn id="8" name="False Positive Rate" dataDxfId="44"/>
+    <tableColumn id="9" name="Score" dataDxfId="43"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Table26412" displayName="Table26412" ref="A2:I4" totalsRowShown="0" tableBorderDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Table26412" displayName="Table26412" ref="A2:I4" totalsRowShown="0" tableBorderDxfId="42">
   <autoFilter ref="A2:I4"/>
   <tableColumns count="9">
     <tableColumn id="1" name="XQuery Library"/>
@@ -3904,16 +4090,16 @@
     <tableColumn id="4" name="True Negative"/>
     <tableColumn id="5" name="False Positive"/>
     <tableColumn id="6" name="Total"/>
-    <tableColumn id="7" name="True Posistive Rate" dataDxfId="6"/>
-    <tableColumn id="8" name="False Positive Rate" dataDxfId="5"/>
-    <tableColumn id="9" name="Score" dataDxfId="4"/>
+    <tableColumn id="7" name="True Posistive Rate" dataDxfId="41"/>
+    <tableColumn id="8" name="False Positive Rate" dataDxfId="40"/>
+    <tableColumn id="9" name="Score" dataDxfId="39"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table28" displayName="Table28" ref="A2:I11" totalsRowShown="0" tableBorderDxfId="56">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table28" displayName="Table28" ref="A2:I11" totalsRowShown="0" tableBorderDxfId="38">
   <autoFilter ref="A2:I11"/>
   <tableColumns count="9">
     <tableColumn id="1" name="XML Parser"/>
@@ -3922,16 +4108,16 @@
     <tableColumn id="4" name="True Negative"/>
     <tableColumn id="5" name="False Positive"/>
     <tableColumn id="6" name="Total"/>
-    <tableColumn id="7" name="True Posistive Rate" dataDxfId="55"/>
-    <tableColumn id="8" name="False Positive Rate" dataDxfId="54"/>
-    <tableColumn id="9" name="Score" dataDxfId="53"/>
+    <tableColumn id="7" name="True Posistive Rate" dataDxfId="37"/>
+    <tableColumn id="8" name="False Positive Rate" dataDxfId="36"/>
+    <tableColumn id="9" name="Score" dataDxfId="35"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table279" displayName="Table279" ref="A30:I39" totalsRowShown="0" tableBorderDxfId="52">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table279" displayName="Table279" ref="A30:I39" totalsRowShown="0" tableBorderDxfId="34">
   <autoFilter ref="A30:I39"/>
   <tableColumns count="9">
     <tableColumn id="1" name="XML Parser"/>
@@ -3940,16 +4126,16 @@
     <tableColumn id="4" name="True Negative"/>
     <tableColumn id="5" name="False Positive"/>
     <tableColumn id="6" name="Total"/>
-    <tableColumn id="7" name="True Posistive Rate" dataDxfId="51"/>
-    <tableColumn id="8" name="False Positive Rate" dataDxfId="50"/>
-    <tableColumn id="9" name="Score" dataDxfId="49"/>
+    <tableColumn id="7" name="True Posistive Rate" dataDxfId="33"/>
+    <tableColumn id="8" name="False Positive Rate" dataDxfId="32"/>
+    <tableColumn id="9" name="Score" dataDxfId="31"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Table2610" displayName="Table2610" ref="A2:I5" totalsRowShown="0" tableBorderDxfId="48">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Table2610" displayName="Table2610" ref="A2:I5" totalsRowShown="0" tableBorderDxfId="30">
   <autoFilter ref="A2:I5"/>
   <tableColumns count="9">
     <tableColumn id="1" name="Query Type"/>
@@ -3958,9 +4144,9 @@
     <tableColumn id="4" name="True Negative"/>
     <tableColumn id="5" name="False Positive"/>
     <tableColumn id="6" name="Total"/>
-    <tableColumn id="7" name="True Posistive Rate" dataDxfId="47"/>
-    <tableColumn id="8" name="False Positive Rate" dataDxfId="46"/>
-    <tableColumn id="9" name="Score" dataDxfId="45"/>
+    <tableColumn id="7" name="True Posistive Rate" dataDxfId="29"/>
+    <tableColumn id="8" name="False Positive Rate" dataDxfId="28"/>
+    <tableColumn id="9" name="Score" dataDxfId="27"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4258,9 +4444,9 @@
   </sheetPr>
   <dimension ref="A1:I58"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B35" sqref="B35"/>
+    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4531,7 +4717,7 @@
         <v>84</v>
       </c>
       <c r="H9" s="10" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I9" s="1" t="s">
         <v>31</v>
@@ -4734,7 +4920,7 @@
         <v>84</v>
       </c>
       <c r="H16" s="10" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I16" s="1" t="s">
         <v>38</v>
@@ -4860,7 +5046,7 @@
       <c r="A21" s="10">
         <v>20</v>
       </c>
-      <c r="B21" s="23" t="s">
+      <c r="B21" s="19" t="s">
         <v>115</v>
       </c>
       <c r="C21" s="11" t="s">
@@ -4889,7 +5075,7 @@
       <c r="A22" s="10">
         <v>21</v>
       </c>
-      <c r="B22" s="23" t="s">
+      <c r="B22" s="19" t="s">
         <v>115</v>
       </c>
       <c r="C22" s="11" t="s">
@@ -4918,7 +5104,7 @@
       <c r="A23" s="10">
         <v>22</v>
       </c>
-      <c r="B23" s="23" t="s">
+      <c r="B23" s="19" t="s">
         <v>115</v>
       </c>
       <c r="C23" s="11" t="s">
@@ -4937,7 +5123,7 @@
         <v>85</v>
       </c>
       <c r="H23" s="16" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I23" s="1" t="s">
         <v>66</v>
@@ -4947,7 +5133,7 @@
       <c r="A24" s="10">
         <v>23</v>
       </c>
-      <c r="B24" s="23" t="s">
+      <c r="B24" s="19" t="s">
         <v>115</v>
       </c>
       <c r="C24" s="11" t="s">
@@ -4966,7 +5152,7 @@
         <v>85</v>
       </c>
       <c r="H24" s="16" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I24" s="1" t="s">
         <v>67</v>
@@ -4976,7 +5162,7 @@
       <c r="A25" s="10">
         <v>24</v>
       </c>
-      <c r="B25" s="23" t="s">
+      <c r="B25" s="19" t="s">
         <v>115</v>
       </c>
       <c r="C25" s="11" t="s">
@@ -4995,7 +5181,7 @@
         <v>85</v>
       </c>
       <c r="H25" s="16" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I25" s="1" t="s">
         <v>68</v>
@@ -5005,7 +5191,7 @@
       <c r="A26" s="10">
         <v>25</v>
       </c>
-      <c r="B26" s="23" t="s">
+      <c r="B26" s="19" t="s">
         <v>115</v>
       </c>
       <c r="C26" s="11" t="s">
@@ -5034,7 +5220,7 @@
       <c r="A27" s="10">
         <v>26</v>
       </c>
-      <c r="B27" s="23" t="s">
+      <c r="B27" s="19" t="s">
         <v>115</v>
       </c>
       <c r="C27" s="11" t="s">
@@ -5063,7 +5249,7 @@
       <c r="A28" s="10">
         <v>27</v>
       </c>
-      <c r="B28" s="23" t="s">
+      <c r="B28" s="19" t="s">
         <v>115</v>
       </c>
       <c r="C28" s="11" t="s">
@@ -5082,7 +5268,7 @@
         <v>85</v>
       </c>
       <c r="H28" s="16" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I28" s="1" t="s">
         <v>72</v>
@@ -5092,7 +5278,7 @@
       <c r="A29" s="10">
         <v>28</v>
       </c>
-      <c r="B29" s="23" t="s">
+      <c r="B29" s="19" t="s">
         <v>115</v>
       </c>
       <c r="C29" s="11" t="s">
@@ -5111,7 +5297,7 @@
         <v>85</v>
       </c>
       <c r="H29" s="16" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I29" s="1" t="s">
         <v>76</v>
@@ -5121,7 +5307,7 @@
       <c r="A30" s="10">
         <v>29</v>
       </c>
-      <c r="B30" s="23" t="s">
+      <c r="B30" s="19" t="s">
         <v>115</v>
       </c>
       <c r="C30" s="11" t="s">
@@ -5226,8 +5412,8 @@
       <c r="G33" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="H33" s="10" t="s">
-        <v>85</v>
+      <c r="H33" s="18" t="s">
+        <v>84</v>
       </c>
       <c r="I33" s="1" t="s">
         <v>146</v>
@@ -5512,122 +5698,122 @@
       <c r="C58" s="2"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="G16:H16 G9:H13 G2:H6 G20:H20 F2:F20 H7:H20 G33:H39">
-    <cfRule type="containsText" dxfId="40" priority="28" operator="containsText" text="Safe">
+  <conditionalFormatting sqref="G16:H16 G9:H13 G2:H6 G20:H20 F2:F20 H7:H20 G34:H39 G33">
+    <cfRule type="containsText" dxfId="91" priority="28" operator="containsText" text="Safe">
       <formula>NOT(ISERROR(SEARCH("Safe",F2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="39" priority="29" operator="containsText" text="Safe">
+    <cfRule type="containsText" dxfId="90" priority="29" operator="containsText" text="Safe">
       <formula>NOT(ISERROR(SEARCH("Safe",F2)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F2:H20 G33:H39">
-    <cfRule type="containsText" dxfId="38" priority="26" operator="containsText" text="Unsafe">
+  <conditionalFormatting sqref="F2:H20 G34:H39 G33">
+    <cfRule type="containsText" dxfId="89" priority="26" operator="containsText" text="Unsafe">
       <formula>NOT(ISERROR(SEARCH("Unsafe",F2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="37" priority="27" operator="containsText" text="Safe">
+    <cfRule type="containsText" dxfId="88" priority="27" operator="containsText" text="Safe">
       <formula>NOT(ISERROR(SEARCH("Safe",F2)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E40:F1048576 G1:H20 G33:H39">
-    <cfRule type="containsText" dxfId="36" priority="24" operator="containsText" text="Fail">
+  <conditionalFormatting sqref="E40:F1048576 G1:H20 G34:H39 G33">
+    <cfRule type="containsText" dxfId="87" priority="24" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="35" priority="25" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="86" priority="25" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",E1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F1:H20 F40:H1048576 G33:H39">
-    <cfRule type="containsText" dxfId="34" priority="23" operator="containsText" text="4.5.2">
+  <conditionalFormatting sqref="F1:H20 F40:H1048576 G34:H39 G33">
+    <cfRule type="containsText" dxfId="85" priority="23" operator="containsText" text="4.5.2">
       <formula>NOT(ISERROR(SEARCH("4.5.2",F1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F21:H27">
-    <cfRule type="containsText" dxfId="33" priority="19" operator="containsText" text="Unsafe">
+  <conditionalFormatting sqref="F21:H27 H28:H29">
+    <cfRule type="containsText" dxfId="84" priority="19" operator="containsText" text="Unsafe">
       <formula>NOT(ISERROR(SEARCH("Unsafe",F21)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="32" priority="20" operator="containsText" text="Safe">
+    <cfRule type="containsText" dxfId="83" priority="20" operator="containsText" text="Safe">
       <formula>NOT(ISERROR(SEARCH("Safe",F21)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F21:H27">
-    <cfRule type="containsText" dxfId="31" priority="21" operator="containsText" text="Safe">
+  <conditionalFormatting sqref="F21:H27 H28:H29">
+    <cfRule type="containsText" dxfId="82" priority="21" operator="containsText" text="Safe">
       <formula>NOT(ISERROR(SEARCH("Safe",F21)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="30" priority="22" operator="containsText" text="Safe">
+    <cfRule type="containsText" dxfId="81" priority="22" operator="containsText" text="Safe">
       <formula>NOT(ISERROR(SEARCH("Safe",F21)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G21:G27 H21">
-    <cfRule type="containsText" dxfId="29" priority="18" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="80" priority="18" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",G21)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G21:H27">
-    <cfRule type="containsText" dxfId="28" priority="16" operator="containsText" text="Fail">
+  <conditionalFormatting sqref="G21:H27 H28:H29">
+    <cfRule type="containsText" dxfId="79" priority="16" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",G21)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="27" priority="17" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="78" priority="17" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",G21)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F28:H30 G31:H32">
-    <cfRule type="containsText" dxfId="26" priority="12" operator="containsText" text="Unsafe">
+  <conditionalFormatting sqref="F30:H30 G31:H32 F28:G29 H33">
+    <cfRule type="containsText" dxfId="77" priority="12" operator="containsText" text="Unsafe">
       <formula>NOT(ISERROR(SEARCH("Unsafe",F28)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="25" priority="13" operator="containsText" text="Safe">
+    <cfRule type="containsText" dxfId="76" priority="13" operator="containsText" text="Safe">
       <formula>NOT(ISERROR(SEARCH("Safe",F28)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F28:H30 G31:H32">
-    <cfRule type="containsText" dxfId="24" priority="14" operator="containsText" text="Safe">
+  <conditionalFormatting sqref="F30:H30 G31:H32 F28:G29 H33">
+    <cfRule type="containsText" dxfId="75" priority="14" operator="containsText" text="Safe">
       <formula>NOT(ISERROR(SEARCH("Safe",F28)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="23" priority="15" operator="containsText" text="Safe">
+    <cfRule type="containsText" dxfId="74" priority="15" operator="containsText" text="Safe">
       <formula>NOT(ISERROR(SEARCH("Safe",F28)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G28:G32 H31:H32">
-    <cfRule type="containsText" dxfId="22" priority="11" operator="containsText" text="Pass">
+  <conditionalFormatting sqref="G28:G32 H31:H33">
+    <cfRule type="containsText" dxfId="73" priority="11" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",G28)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G28:H32">
-    <cfRule type="containsText" dxfId="21" priority="9" operator="containsText" text="Fail">
+  <conditionalFormatting sqref="G30:H32 G28:G29 H33">
+    <cfRule type="containsText" dxfId="72" priority="9" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",G28)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="20" priority="10" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="71" priority="10" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",G28)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F31:F34">
-    <cfRule type="containsText" dxfId="19" priority="5" operator="containsText" text="Unsafe">
+    <cfRule type="containsText" dxfId="70" priority="5" operator="containsText" text="Unsafe">
       <formula>NOT(ISERROR(SEARCH("Unsafe",F31)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="18" priority="6" operator="containsText" text="Safe">
+    <cfRule type="containsText" dxfId="69" priority="6" operator="containsText" text="Safe">
       <formula>NOT(ISERROR(SEARCH("Safe",F31)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F31:F34">
-    <cfRule type="containsText" dxfId="17" priority="7" operator="containsText" text="Safe">
+    <cfRule type="containsText" dxfId="68" priority="7" operator="containsText" text="Safe">
       <formula>NOT(ISERROR(SEARCH("Safe",F31)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="16" priority="8" operator="containsText" text="Safe">
+    <cfRule type="containsText" dxfId="67" priority="8" operator="containsText" text="Safe">
       <formula>NOT(ISERROR(SEARCH("Safe",F31)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F35:F39">
-    <cfRule type="containsText" dxfId="15" priority="1" operator="containsText" text="Unsafe">
+    <cfRule type="containsText" dxfId="66" priority="1" operator="containsText" text="Unsafe">
       <formula>NOT(ISERROR(SEARCH("Unsafe",F35)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="14" priority="2" operator="containsText" text="Safe">
+    <cfRule type="containsText" dxfId="65" priority="2" operator="containsText" text="Safe">
       <formula>NOT(ISERROR(SEARCH("Safe",F35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F35:F39">
-    <cfRule type="containsText" dxfId="13" priority="3" operator="containsText" text="Safe">
+    <cfRule type="containsText" dxfId="64" priority="3" operator="containsText" text="Safe">
       <formula>NOT(ISERROR(SEARCH("Safe",F35)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="4" operator="containsText" text="Safe">
+    <cfRule type="containsText" dxfId="63" priority="4" operator="containsText" text="Safe">
       <formula>NOT(ISERROR(SEARCH("Safe",F35)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5662,17 +5848,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
@@ -5702,7 +5888,7 @@
       <c r="I2" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="K2" s="20" t="s">
+      <c r="K2" s="21" t="s">
         <v>53</v>
       </c>
     </row>
@@ -5734,7 +5920,7 @@
         <f>(Table2[[#This Row],[True Posistive Rate]]+(1 - Table2[[#This Row],[False Positive Rate]])) - 1</f>
         <v>1</v>
       </c>
-      <c r="K3" s="21"/>
+      <c r="K3" s="22"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
@@ -5764,7 +5950,7 @@
         <f>(Table2[[#This Row],[True Posistive Rate]]+(1 - Table2[[#This Row],[False Positive Rate]])) - 1</f>
         <v>1</v>
       </c>
-      <c r="K4" s="21"/>
+      <c r="K4" s="22"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
@@ -5794,7 +5980,7 @@
         <f>(Table2[[#This Row],[True Posistive Rate]]+(1 - Table2[[#This Row],[False Positive Rate]])) - 1</f>
         <v>1</v>
       </c>
-      <c r="K5" s="21"/>
+      <c r="K5" s="22"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
@@ -5824,7 +6010,7 @@
         <f>(Table2[[#This Row],[True Posistive Rate]]+(1 - Table2[[#This Row],[False Positive Rate]])) - 1</f>
         <v>1</v>
       </c>
-      <c r="K6" s="21"/>
+      <c r="K6" s="22"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
@@ -5854,7 +6040,7 @@
         <f>(Table2[[#This Row],[True Posistive Rate]]+(1 - Table2[[#This Row],[False Positive Rate]])) - 1</f>
         <v>1</v>
       </c>
-      <c r="K7" s="21"/>
+      <c r="K7" s="22"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
@@ -5884,7 +6070,7 @@
         <f>(Table2[[#This Row],[True Posistive Rate]]+(1 - Table2[[#This Row],[False Positive Rate]])) - 1</f>
         <v>1</v>
       </c>
-      <c r="K8" s="21"/>
+      <c r="K8" s="22"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
@@ -5914,7 +6100,7 @@
         <f>(Table2[[#This Row],[True Posistive Rate]]+(1 - Table2[[#This Row],[False Positive Rate]])) - 1</f>
         <v>1</v>
       </c>
-      <c r="K9" s="21"/>
+      <c r="K9" s="22"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
@@ -5944,7 +6130,7 @@
         <f>(Table2[[#This Row],[True Posistive Rate]]+(1 - Table2[[#This Row],[False Positive Rate]])) - 1</f>
         <v>0</v>
       </c>
-      <c r="K10" s="21"/>
+      <c r="K10" s="22"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
@@ -5982,7 +6168,7 @@
         <f>ROUND(AVERAGE(I3:I10)*100, 0)</f>
         <v>88</v>
       </c>
-      <c r="K11" s="21"/>
+      <c r="K11" s="22"/>
     </row>
     <row r="12" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="10"/>
@@ -6152,17 +6338,17 @@
       <c r="I27" s="9"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="19" t="s">
+      <c r="A29" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="B29" s="19"/>
-      <c r="C29" s="19"/>
-      <c r="D29" s="19"/>
-      <c r="E29" s="19"/>
-      <c r="F29" s="19"/>
-      <c r="G29" s="19"/>
-      <c r="H29" s="19"/>
-      <c r="I29" s="19"/>
+      <c r="B29" s="20"/>
+      <c r="C29" s="20"/>
+      <c r="D29" s="20"/>
+      <c r="E29" s="20"/>
+      <c r="F29" s="20"/>
+      <c r="G29" s="20"/>
+      <c r="H29" s="20"/>
+      <c r="I29" s="20"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="10" t="s">
@@ -6662,7 +6848,7 @@
   <dimension ref="A1:K28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I22" sqref="A1:I22"/>
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6680,17 +6866,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="23" t="s">
         <v>81</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
@@ -6721,7 +6907,7 @@
         <v>50</v>
       </c>
       <c r="J2" s="10"/>
-      <c r="K2" s="20" t="s">
+      <c r="K2" s="21" t="s">
         <v>79</v>
       </c>
     </row>
@@ -6754,7 +6940,7 @@
         <v>0</v>
       </c>
       <c r="J3" s="10"/>
-      <c r="K3" s="21"/>
+      <c r="K3" s="22"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
@@ -6785,7 +6971,7 @@
         <v>0</v>
       </c>
       <c r="J4" s="10"/>
-      <c r="K4" s="21"/>
+      <c r="K4" s="22"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
@@ -6824,7 +7010,7 @@
         <v>0</v>
       </c>
       <c r="J5" s="10"/>
-      <c r="K5" s="21"/>
+      <c r="K5" s="22"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="10"/>
@@ -6837,7 +7023,7 @@
       <c r="H6" s="10"/>
       <c r="I6" s="10"/>
       <c r="J6" s="10"/>
-      <c r="K6" s="21"/>
+      <c r="K6" s="22"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="10"/>
@@ -6850,7 +7036,7 @@
       <c r="H7" s="10"/>
       <c r="I7" s="10"/>
       <c r="J7" s="10"/>
-      <c r="K7" s="21"/>
+      <c r="K7" s="22"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="10"/>
@@ -6863,7 +7049,7 @@
       <c r="H8" s="10"/>
       <c r="I8" s="10"/>
       <c r="J8" s="10"/>
-      <c r="K8" s="21"/>
+      <c r="K8" s="22"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="10"/>
@@ -6876,7 +7062,7 @@
       <c r="H9" s="10"/>
       <c r="I9" s="10"/>
       <c r="J9" s="10"/>
-      <c r="K9" s="21"/>
+      <c r="K9" s="22"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="10"/>
@@ -6889,7 +7075,7 @@
       <c r="H10" s="10"/>
       <c r="I10" s="10"/>
       <c r="J10" s="10"/>
-      <c r="K10" s="21"/>
+      <c r="K10" s="22"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="10"/>
@@ -6902,7 +7088,7 @@
       <c r="H11" s="10"/>
       <c r="I11" s="10"/>
       <c r="J11" s="10"/>
-      <c r="K11" s="21"/>
+      <c r="K11" s="22"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="10"/>
@@ -7106,17 +7292,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="23" t="s">
         <v>110</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
@@ -7434,17 +7620,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="23" t="s">
         <v>111</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
@@ -7744,8 +7930,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K55"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D41" sqref="D41"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D45" sqref="D45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7763,17 +7949,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
       <c r="J1" s="10"/>
       <c r="K1" s="10"/>
     </row>
@@ -7806,7 +7992,7 @@
         <v>50</v>
       </c>
       <c r="J2" s="10"/>
-      <c r="K2" s="20" t="s">
+      <c r="K2" s="21" t="s">
         <v>86</v>
       </c>
     </row>
@@ -7839,7 +8025,7 @@
         <v>1</v>
       </c>
       <c r="J3" s="10"/>
-      <c r="K3" s="21"/>
+      <c r="K3" s="22"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
@@ -7870,7 +8056,7 @@
         <v>1</v>
       </c>
       <c r="J4" s="10"/>
-      <c r="K4" s="21"/>
+      <c r="K4" s="22"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
@@ -7901,7 +8087,7 @@
         <v>0</v>
       </c>
       <c r="J5" s="10"/>
-      <c r="K5" s="21"/>
+      <c r="K5" s="22"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
@@ -7930,7 +8116,7 @@
         <v>0</v>
       </c>
       <c r="J6" s="10"/>
-      <c r="K6" s="21"/>
+      <c r="K6" s="22"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
@@ -7961,7 +8147,7 @@
         <v>1</v>
       </c>
       <c r="J7" s="10"/>
-      <c r="K7" s="21"/>
+      <c r="K7" s="22"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
@@ -7992,7 +8178,7 @@
         <v>0</v>
       </c>
       <c r="J8" s="10"/>
-      <c r="K8" s="21"/>
+      <c r="K8" s="22"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
@@ -8023,7 +8209,7 @@
         <v>0</v>
       </c>
       <c r="J9" s="10"/>
-      <c r="K9" s="21"/>
+      <c r="K9" s="22"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
@@ -8054,7 +8240,7 @@
         <v>1</v>
       </c>
       <c r="J10" s="10"/>
-      <c r="K10" s="21"/>
+      <c r="K10" s="22"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
@@ -8093,7 +8279,7 @@
         <v>50</v>
       </c>
       <c r="J11" s="10"/>
-      <c r="K11" s="21"/>
+      <c r="K11" s="22"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="10"/>
@@ -8317,17 +8503,17 @@
       <c r="K28" s="10"/>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="19" t="s">
+      <c r="A29" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="B29" s="19"/>
-      <c r="C29" s="19"/>
-      <c r="D29" s="19"/>
-      <c r="E29" s="19"/>
-      <c r="F29" s="19"/>
-      <c r="G29" s="19"/>
-      <c r="H29" s="19"/>
-      <c r="I29" s="19"/>
+      <c r="B29" s="20"/>
+      <c r="C29" s="20"/>
+      <c r="D29" s="20"/>
+      <c r="E29" s="20"/>
+      <c r="F29" s="20"/>
+      <c r="G29" s="20"/>
+      <c r="H29" s="20"/>
+      <c r="I29" s="20"/>
       <c r="J29" s="10"/>
       <c r="K29" s="10"/>
     </row>
@@ -8519,10 +8705,10 @@
       <c r="A36" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="B36" s="10"/>
-      <c r="C36" s="10">
-        <v>1</v>
-      </c>
+      <c r="B36" s="10">
+        <v>1</v>
+      </c>
+      <c r="C36" s="10"/>
       <c r="D36" s="10">
         <v>2</v>
       </c>
@@ -8533,7 +8719,7 @@
       </c>
       <c r="G36" s="12">
         <f>IF(Table279[[#This Row],[True Positive]]+Table279[[#This Row],[False Negative]]=0,0,Table279[[#This Row],[True Positive]]/(Table279[[#This Row],[True Positive]]+Table279[[#This Row],[False Negative]]))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H36" s="12">
         <f>Table279[[#This Row],[False Positive]]/(Table279[[#This Row],[False Positive]]+Table279[[#This Row],[True Negative]])</f>
@@ -8541,7 +8727,7 @@
       </c>
       <c r="I36" s="12">
         <f>(Table279[[#This Row],[True Posistive Rate]]+(1 - Table279[[#This Row],[False Positive Rate]])) - 1</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J36" s="10"/>
       <c r="K36" s="10"/>
@@ -8612,11 +8798,11 @@
       </c>
       <c r="B39" s="8">
         <f>SUM(B31:B38)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C39" s="8">
         <f t="shared" ref="C39:F39" si="1">SUM(C31:C38)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D39" s="8">
         <f t="shared" si="1"/>
@@ -8632,7 +8818,7 @@
       </c>
       <c r="G39" s="8">
         <f>AVERAGE(G31:G38)</f>
-        <v>0.625</v>
+        <v>0.75</v>
       </c>
       <c r="H39" s="8">
         <f>AVERAGE(H31:H38)</f>
@@ -8640,7 +8826,7 @@
       </c>
       <c r="I39" s="8">
         <f>ROUND(AVERAGE(I31:I38)*100, 0)</f>
-        <v>63</v>
+        <v>75</v>
       </c>
       <c r="J39" s="10"/>
       <c r="K39" s="10"/>
@@ -8873,7 +9059,7 @@
   <dimension ref="A1:K21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8890,17 +9076,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="23" t="s">
         <v>80</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
       <c r="J1" s="10"/>
       <c r="K1" s="10"/>
     </row>
@@ -8933,18 +9119,16 @@
         <v>50</v>
       </c>
       <c r="J2" s="10"/>
-      <c r="K2" s="20"/>
+      <c r="K2" s="21"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
         <v>56</v>
       </c>
       <c r="B3" s="10">
-        <v>1</v>
-      </c>
-      <c r="C3" s="10">
-        <v>3</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="C3" s="10"/>
       <c r="D3" s="10">
         <v>3</v>
       </c>
@@ -8955,7 +9139,7 @@
       </c>
       <c r="G3" s="12">
         <f>IF(Table2610[[#This Row],[True Positive]]+Table2610[[#This Row],[False Negative]]=0,0,Table2610[[#This Row],[True Positive]]/(Table2610[[#This Row],[True Positive]]+Table2610[[#This Row],[False Negative]]))</f>
-        <v>0.25</v>
+        <v>1</v>
       </c>
       <c r="H3" s="12">
         <f>Table2610[[#This Row],[False Positive]]/(Table2610[[#This Row],[False Positive]]+Table2610[[#This Row],[True Negative]])</f>
@@ -8963,19 +9147,19 @@
       </c>
       <c r="I3" s="12">
         <f>(Table2610[[#This Row],[True Posistive Rate]]+(1 - Table2610[[#This Row],[False Positive Rate]])) - 1</f>
-        <v>0.25</v>
+        <v>1</v>
       </c>
       <c r="J3" s="10"/>
-      <c r="K3" s="21"/>
+      <c r="K3" s="22"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="B4" s="10"/>
-      <c r="C4" s="10">
+      <c r="B4" s="10">
         <v>2</v>
       </c>
+      <c r="C4" s="10"/>
       <c r="D4" s="10">
         <v>1</v>
       </c>
@@ -8986,7 +9170,7 @@
       </c>
       <c r="G4" s="12">
         <f>IF(Table2610[[#This Row],[True Positive]]+Table2610[[#This Row],[False Negative]]=0,0,Table2610[[#This Row],[True Positive]]/(Table2610[[#This Row],[True Positive]]+Table2610[[#This Row],[False Negative]]))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H4" s="12">
         <f>Table2610[[#This Row],[False Positive]]/(Table2610[[#This Row],[False Positive]]+Table2610[[#This Row],[True Negative]])</f>
@@ -8994,10 +9178,10 @@
       </c>
       <c r="I4" s="12">
         <f>(Table2610[[#This Row],[True Posistive Rate]]+(1 - Table2610[[#This Row],[False Positive Rate]])) - 1</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J4" s="10"/>
-      <c r="K4" s="21"/>
+      <c r="K4" s="22"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
@@ -9005,11 +9189,11 @@
       </c>
       <c r="B5" s="8">
         <f>SUM(B3:B4)</f>
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C5" s="8">
         <f>SUM(C3:C4)</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D5" s="8">
         <f>SUM(D3:D4)</f>
@@ -9025,7 +9209,7 @@
       </c>
       <c r="G5" s="8">
         <f>AVERAGE(G3:G4)</f>
-        <v>0.125</v>
+        <v>1</v>
       </c>
       <c r="H5" s="8">
         <f>AVERAGE(H3:H4)</f>
@@ -9033,10 +9217,10 @@
       </c>
       <c r="I5" s="8">
         <f>ROUND(AVERAGE(I3:I4)*100, 0)</f>
-        <v>13</v>
+        <v>100</v>
       </c>
       <c r="J5" s="10"/>
-      <c r="K5" s="21"/>
+      <c r="K5" s="22"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="10"/>
@@ -9049,7 +9233,7 @@
       <c r="H6" s="10"/>
       <c r="I6" s="10"/>
       <c r="J6" s="10"/>
-      <c r="K6" s="21"/>
+      <c r="K6" s="22"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="10"/>
@@ -9062,7 +9246,7 @@
       <c r="H7" s="10"/>
       <c r="I7" s="10"/>
       <c r="J7" s="10"/>
-      <c r="K7" s="21"/>
+      <c r="K7" s="22"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="10"/>
@@ -9075,7 +9259,7 @@
       <c r="H8" s="10"/>
       <c r="I8" s="10"/>
       <c r="J8" s="10"/>
-      <c r="K8" s="21"/>
+      <c r="K8" s="22"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="10"/>
@@ -9088,7 +9272,7 @@
       <c r="H9" s="10"/>
       <c r="I9" s="10"/>
       <c r="J9" s="10"/>
-      <c r="K9" s="21"/>
+      <c r="K9" s="22"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="10"/>
@@ -9101,7 +9285,7 @@
       <c r="H10" s="10"/>
       <c r="I10" s="10"/>
       <c r="J10" s="10"/>
-      <c r="K10" s="21"/>
+      <c r="K10" s="22"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="10"/>
@@ -9114,7 +9298,7 @@
       <c r="H11" s="10"/>
       <c r="I11" s="10"/>
       <c r="J11" s="10"/>
-      <c r="K11" s="21"/>
+      <c r="K11" s="22"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="10"/>
@@ -9263,8 +9447,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9282,17 +9466,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="23" t="s">
         <v>110</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
@@ -9330,7 +9514,7 @@
       <c r="B3" s="10">
         <v>3</v>
       </c>
-      <c r="E3" s="10">
+      <c r="D3" s="10">
         <v>1</v>
       </c>
       <c r="F3" s="10">
@@ -9343,11 +9527,11 @@
       </c>
       <c r="H3" s="12">
         <f>Table26411[[#This Row],[False Positive]]/(Table26411[[#This Row],[False Positive]]+Table26411[[#This Row],[True Negative]])</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I3" s="12">
         <f>(Table26411[[#This Row],[True Posistive Rate]]+(1 - Table26411[[#This Row],[False Positive Rate]])) - 1</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -9364,11 +9548,11 @@
       </c>
       <c r="D4" s="8">
         <f>SUM(D3:D3)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E4" s="8">
         <f>SUM(E3:E3)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F4" s="8">
         <f>SUM(F3:F3)</f>
@@ -9380,11 +9564,11 @@
       </c>
       <c r="H4" s="8">
         <f>AVERAGE(H3:H3)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I4" s="8">
         <f>ROUND(AVERAGE(I3:I3)*100, 0)</f>
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -9425,17 +9609,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="23" t="s">
         <v>111</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">

</xml_diff>